<commit_message>
Update scripts and functions for result analysis
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -314,6 +314,26 @@
   </si>
   <si>
     <t>long_test_22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_27</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -366,7 +386,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -384,6 +404,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,13 +702,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z59"/>
+  <dimension ref="A1:AE59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="T15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X16" sqref="X16"/>
+      <selection pane="bottomRight" activeCell="AE26" sqref="AE26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -698,7 +721,7 @@
     <col min="24" max="24" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
+    <row r="1" spans="1:31" s="1" customFormat="1">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -772,8 +795,23 @@
       <c r="Z1" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="AA1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -781,7 +819,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:31">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -861,7 +899,7 @@
         <v>2.94</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:31">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -938,7 +976,7 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:31">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1053,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:31">
       <c r="C6">
         <v>1.1000000000000001</v>
       </c>
@@ -1089,7 +1127,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:31">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1166,7 +1204,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:31">
       <c r="C8">
         <v>6.11</v>
       </c>
@@ -1240,7 +1278,7 @@
         <v>3.31</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:31">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1317,7 +1355,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:31">
       <c r="C10">
         <v>4.07</v>
       </c>
@@ -1391,7 +1429,7 @@
         <v>5.96</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:31">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1432,7 +1470,7 @@
         <v>91.8</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:31">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -1470,7 +1508,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:31">
       <c r="E13" s="2">
         <v>41.75</v>
       </c>
@@ -1493,7 +1531,7 @@
         <v>92.4</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:31">
       <c r="E14" s="2">
         <v>1.0780000000000001</v>
       </c>
@@ -1516,7 +1554,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:31">
       <c r="K15">
         <v>72.5</v>
       </c>
@@ -1524,7 +1562,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:31">
       <c r="K16">
         <v>1.2</v>
       </c>
@@ -1532,12 +1570,12 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:31">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:31">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1550,16 +1588,34 @@
       <c r="F18">
         <v>5.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="AA18">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="AB18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AD18">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="AE18">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D19">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="AA19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AC19">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1569,16 +1625,34 @@
       <c r="F20">
         <v>1.2999999999999999E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="AA20">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="AB20">
+        <v>1E-3</v>
+      </c>
+      <c r="AD20">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="AE20">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D21">
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="AA21">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AC21">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1588,32 +1662,56 @@
       <c r="F22">
         <v>4.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="AA22">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="AB22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AE22">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="D23">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F23">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="AA23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="D24">
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="F24">
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="AA24">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AB24">
+        <v>1E-3</v>
+      </c>
+      <c r="AE24">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="D25">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F25">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="AA25">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
@@ -1623,32 +1721,56 @@
       <c r="F26" s="2">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="AA26" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="AB26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AE26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="D27">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F27" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="AA27" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="D28">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F28" s="2">
         <v>2.5000000000000001E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="AA28" s="2">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AB28">
+        <v>1.75E-4</v>
+      </c>
+      <c r="AE28">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="D29">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F29" s="2">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="AA29" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="B30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1658,27 +1780,39 @@
       <c r="F30" s="2">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="AA30" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="D31">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="AA31" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="D32">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F32" s="2">
         <v>1.75E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="AA32" s="2">
+        <v>1.75E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
       <c r="D33">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="AA33">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -1700,8 +1834,11 @@
       <c r="W35">
         <v>1.95</v>
       </c>
-    </row>
-    <row r="36" spans="1:24">
+      <c r="AA35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
       <c r="B36" s="3" t="s">
         <v>5</v>
       </c>
@@ -1717,8 +1854,11 @@
       <c r="W36">
         <v>1.46</v>
       </c>
-    </row>
-    <row r="37" spans="1:24">
+      <c r="AA36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
@@ -1740,8 +1880,11 @@
       <c r="Q37">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="AA37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29">
       <c r="B38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1763,8 +1906,11 @@
       <c r="Q38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:24">
+      <c r="AA38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29">
       <c r="C39" t="s">
         <v>32</v>
       </c>
@@ -1772,7 +1918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:29">
       <c r="A40" s="3" t="s">
         <v>16</v>
       </c>
@@ -1782,26 +1928,23 @@
       <c r="C40">
         <v>1.33</v>
       </c>
-      <c r="D40">
-        <v>3.6</v>
-      </c>
       <c r="M40">
         <v>2.85</v>
       </c>
       <c r="N40">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="AA40">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29">
       <c r="B41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C41">
         <v>0.96199999999999997</v>
       </c>
-      <c r="D41">
-        <v>2.6</v>
-      </c>
       <c r="E41" s="2">
         <v>3.4</v>
       </c>
@@ -1811,42 +1954,45 @@
       <c r="N41">
         <v>3.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:24">
+      <c r="AA41">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29">
       <c r="B42" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C42">
         <v>0.61499999999999999</v>
       </c>
-      <c r="D42">
-        <v>1.5</v>
-      </c>
       <c r="M42">
         <v>1.25</v>
       </c>
       <c r="N42">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="43" spans="1:24">
+      <c r="AA42">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29">
       <c r="B43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C43">
         <v>0.65600000000000003</v>
       </c>
-      <c r="D43">
-        <v>1.6</v>
-      </c>
       <c r="M43">
         <v>1.3</v>
       </c>
       <c r="N43">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="44" spans="1:24">
+      <c r="AA43">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29">
       <c r="B44" s="3" t="s">
         <v>21</v>
       </c>
@@ -1889,8 +2035,11 @@
       <c r="X44" s="5">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="AA44">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29">
       <c r="B45" s="3" t="s">
         <v>22</v>
       </c>
@@ -1933,8 +2082,11 @@
       <c r="X45" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:24">
+      <c r="AA45">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
       <c r="B46" s="3" t="s">
         <v>23</v>
       </c>
@@ -1956,8 +2108,11 @@
       <c r="X46" s="5">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="47" spans="1:24">
+      <c r="AA46">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
       <c r="B47" s="3" t="s">
         <v>24</v>
       </c>
@@ -1979,8 +2134,11 @@
       <c r="X47" s="5">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="48" spans="1:24">
+      <c r="AA47">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
       <c r="B48" s="3" t="s">
         <v>25</v>
       </c>
@@ -2002,8 +2160,14 @@
       <c r="S48">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:24">
+      <c r="AA48">
+        <v>2.4</v>
+      </c>
+      <c r="AC48">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31">
       <c r="B49" s="3" t="s">
         <v>26</v>
       </c>
@@ -2016,8 +2180,11 @@
       <c r="S49">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="50" spans="1:24">
+      <c r="AA49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31">
       <c r="B50" s="3" t="s">
         <v>27</v>
       </c>
@@ -2027,8 +2194,11 @@
       <c r="D50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:24">
+      <c r="AA50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31">
       <c r="B51" s="3" t="s">
         <v>38</v>
       </c>
@@ -2038,8 +2208,11 @@
       <c r="D51">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:24">
+      <c r="AA51">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31">
       <c r="B52" s="3" t="s">
         <v>28</v>
       </c>
@@ -2061,8 +2234,17 @@
       <c r="Q52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:24">
+      <c r="AA52">
+        <v>3</v>
+      </c>
+      <c r="AB52">
+        <v>2</v>
+      </c>
+      <c r="AE52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31">
       <c r="B53" s="3" t="s">
         <v>30</v>
       </c>
@@ -2075,8 +2257,14 @@
       <c r="P53">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="54" spans="1:24">
+      <c r="AA53">
+        <v>1.5</v>
+      </c>
+      <c r="AB53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31">
       <c r="B54" s="3" t="s">
         <v>31</v>
       </c>
@@ -2104,8 +2292,14 @@
       <c r="W54" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="55" spans="1:24">
+      <c r="AA54">
+        <v>1</v>
+      </c>
+      <c r="AC54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31">
       <c r="B55" s="3" t="s">
         <v>29</v>
       </c>
@@ -2118,8 +2312,14 @@
       <c r="P55">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="57" spans="1:24">
+      <c r="AA55">
+        <v>1</v>
+      </c>
+      <c r="AC55">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31">
       <c r="A57" s="3" t="s">
         <v>37</v>
       </c>
@@ -2151,12 +2351,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:31">
       <c r="W58" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:31">
       <c r="W59" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Add functions for analysis;tune network model
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -334,6 +334,54 @@
   </si>
   <si>
     <t>baseline_test_27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>synapse delay decreased</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Syn Decay Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSI2PN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSI2ITN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTS2ITN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTS2PN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>std 0.5*mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>std 0.4*mean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,13 +750,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE59"/>
+  <dimension ref="A1:AJ64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="T15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="Y3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE26" sqref="AE26"/>
+      <selection pane="bottomRight" activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -721,7 +769,7 @@
     <col min="24" max="24" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1">
+    <row r="1" spans="1:36" s="1" customFormat="1">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -810,8 +858,21 @@
       <c r="AE1" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:31">
+      <c r="AF1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ1" s="6"/>
+    </row>
+    <row r="2" spans="1:36">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -819,7 +880,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:36">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -898,8 +959,35 @@
       <c r="Z3">
         <v>2.94</v>
       </c>
-    </row>
-    <row r="4" spans="1:31">
+      <c r="AA3">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AB3">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="AC3">
+        <v>0.42</v>
+      </c>
+      <c r="AD3">
+        <v>1.85</v>
+      </c>
+      <c r="AE3">
+        <v>1.28</v>
+      </c>
+      <c r="AF3">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="AG3">
+        <v>1.65</v>
+      </c>
+      <c r="AH3">
+        <v>1.96</v>
+      </c>
+      <c r="AI3">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -975,8 +1063,35 @@
       <c r="Z4">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:31">
+      <c r="AA4">
+        <v>1.74</v>
+      </c>
+      <c r="AB4">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="AC4">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="AD4">
+        <v>1.68</v>
+      </c>
+      <c r="AE4">
+        <v>1.31</v>
+      </c>
+      <c r="AF4">
+        <v>1.46</v>
+      </c>
+      <c r="AG4">
+        <v>2.1</v>
+      </c>
+      <c r="AH4">
+        <v>2.06</v>
+      </c>
+      <c r="AI4">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1052,8 +1167,35 @@
       <c r="Z5">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="6" spans="1:31">
+      <c r="AA5">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="AB5">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="AC5">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="AD5">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="AE5">
+        <v>1.27</v>
+      </c>
+      <c r="AF5">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="AG5">
+        <v>1.26</v>
+      </c>
+      <c r="AH5">
+        <v>0.371</v>
+      </c>
+      <c r="AI5">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36">
       <c r="C6">
         <v>1.1000000000000001</v>
       </c>
@@ -1126,8 +1268,35 @@
       <c r="Z6">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="7" spans="1:31">
+      <c r="AA6">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="AB6">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="AC6">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AD6">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="AE6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AF6">
+        <v>1.3</v>
+      </c>
+      <c r="AG6">
+        <v>1.61</v>
+      </c>
+      <c r="AH6">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="AI6">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1203,8 +1372,35 @@
       <c r="Z7">
         <v>3.79</v>
       </c>
-    </row>
-    <row r="8" spans="1:31">
+      <c r="AA7">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="AB7">
+        <v>1.84</v>
+      </c>
+      <c r="AC7">
+        <v>2.63</v>
+      </c>
+      <c r="AD7">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="AE7">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AF7">
+        <v>18.7</v>
+      </c>
+      <c r="AG7">
+        <v>7.14</v>
+      </c>
+      <c r="AH7">
+        <v>4.83</v>
+      </c>
+      <c r="AI7">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36">
       <c r="C8">
         <v>6.11</v>
       </c>
@@ -1277,8 +1473,35 @@
       <c r="Z8">
         <v>3.31</v>
       </c>
-    </row>
-    <row r="9" spans="1:31">
+      <c r="AA8">
+        <v>5.76</v>
+      </c>
+      <c r="AB8">
+        <v>2.16</v>
+      </c>
+      <c r="AC8">
+        <v>2.67</v>
+      </c>
+      <c r="AD8">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="AE8">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AF8">
+        <v>11.2</v>
+      </c>
+      <c r="AG8">
+        <v>3.59</v>
+      </c>
+      <c r="AH8">
+        <v>2.89</v>
+      </c>
+      <c r="AI8">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1354,8 +1577,35 @@
       <c r="Z9">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:31">
+      <c r="AA9">
+        <v>1.7</v>
+      </c>
+      <c r="AB9">
+        <v>1.23</v>
+      </c>
+      <c r="AC9">
+        <v>1.31</v>
+      </c>
+      <c r="AD9">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="AE9">
+        <v>2.91</v>
+      </c>
+      <c r="AF9">
+        <v>6.54</v>
+      </c>
+      <c r="AG9">
+        <v>4.57</v>
+      </c>
+      <c r="AH9">
+        <v>3.1</v>
+      </c>
+      <c r="AI9">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36">
       <c r="C10">
         <v>4.07</v>
       </c>
@@ -1428,8 +1678,35 @@
       <c r="Z10">
         <v>5.96</v>
       </c>
-    </row>
-    <row r="11" spans="1:31">
+      <c r="AA10">
+        <v>2.37</v>
+      </c>
+      <c r="AB10">
+        <v>2.15</v>
+      </c>
+      <c r="AC10">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="AD10">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AE10">
+        <v>2.66</v>
+      </c>
+      <c r="AF10">
+        <v>3.99</v>
+      </c>
+      <c r="AG10">
+        <v>3.08</v>
+      </c>
+      <c r="AH10">
+        <v>2.79</v>
+      </c>
+      <c r="AI10">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1469,8 +1746,23 @@
       <c r="W11">
         <v>91.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:31">
+      <c r="AA11">
+        <v>19.2</v>
+      </c>
+      <c r="AB11">
+        <v>23.2</v>
+      </c>
+      <c r="AC11">
+        <v>21.5</v>
+      </c>
+      <c r="AF11">
+        <v>20.2</v>
+      </c>
+      <c r="AG11">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -1507,8 +1799,23 @@
       <c r="W12">
         <v>0.80800000000000005</v>
       </c>
-    </row>
-    <row r="13" spans="1:31">
+      <c r="AA12">
+        <v>1.85</v>
+      </c>
+      <c r="AB12">
+        <v>0.98</v>
+      </c>
+      <c r="AC12">
+        <v>1.46</v>
+      </c>
+      <c r="AF12">
+        <v>1.69</v>
+      </c>
+      <c r="AG12">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36">
       <c r="E13" s="2">
         <v>41.75</v>
       </c>
@@ -1531,7 +1838,7 @@
         <v>92.4</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:36">
       <c r="E14" s="2">
         <v>1.0780000000000001</v>
       </c>
@@ -1554,7 +1861,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:36">
       <c r="K15">
         <v>72.5</v>
       </c>
@@ -1562,7 +1869,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:36">
       <c r="K16">
         <v>1.2</v>
       </c>
@@ -1570,12 +1877,12 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:35">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:35">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -1601,7 +1908,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:35">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -1615,7 +1922,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:35">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1638,7 +1945,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:35">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -1652,7 +1959,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:35">
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1671,8 +1978,14 @@
       <c r="AE22">
         <v>4.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:31">
+      <c r="AH22">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="AI22">
+        <v>4.1999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35">
       <c r="D23">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1683,7 +1996,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:35">
       <c r="D24">
         <v>1.6000000000000001E-3</v>
       </c>
@@ -1699,8 +2012,14 @@
       <c r="AE24">
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:31">
+      <c r="AH24">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AI24">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35">
       <c r="D25">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -1711,7 +2030,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:35">
       <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
@@ -1730,8 +2049,11 @@
       <c r="AE26">
         <v>4.0000000000000002E-4</v>
       </c>
-    </row>
-    <row r="27" spans="1:31">
+      <c r="AH26">
+        <v>3.2000000000000003E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35">
       <c r="D27">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1742,7 +2064,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:35">
       <c r="D28">
         <v>2.9999999999999997E-4</v>
       </c>
@@ -1756,10 +2078,16 @@
         <v>1.75E-4</v>
       </c>
       <c r="AE28">
+        <v>1.75E-4</v>
+      </c>
+      <c r="AF28">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:31">
+      <c r="AH28">
+        <v>8.0000000000000007E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35">
       <c r="D29">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -1769,8 +2097,14 @@
       <c r="AA29" s="2">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:31">
+      <c r="AE29">
+        <v>1E-3</v>
+      </c>
+      <c r="AF29">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35">
       <c r="B30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1783,8 +2117,11 @@
       <c r="AA30" s="2">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:31">
+      <c r="AH30">
+        <v>6.4000000000000005E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35">
       <c r="D31">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -1793,7 +2130,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:35">
       <c r="D32">
         <v>2.0000000000000001E-4</v>
       </c>
@@ -1803,8 +2140,11 @@
       <c r="AA32" s="2">
         <v>1.75E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:29">
+      <c r="AH32">
+        <v>1.6000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35">
       <c r="D33">
         <v>2E-3</v>
       </c>
@@ -1812,7 +2152,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:35">
       <c r="A35" s="3" t="s">
         <v>15</v>
       </c>
@@ -1837,8 +2177,17 @@
       <c r="AA35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:29">
+      <c r="AF35" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH35" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35">
       <c r="B36" s="3" t="s">
         <v>5</v>
       </c>
@@ -1857,8 +2206,17 @@
       <c r="AA36">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:29">
+      <c r="AF36" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35">
       <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
@@ -1883,8 +2241,11 @@
       <c r="AA37">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:29">
+      <c r="AF37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35">
       <c r="B38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1909,8 +2270,11 @@
       <c r="AA38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:29">
+      <c r="AF38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35">
       <c r="C39" t="s">
         <v>32</v>
       </c>
@@ -1918,7 +2282,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:29">
+    <row r="40" spans="1:35">
       <c r="A40" s="3" t="s">
         <v>16</v>
       </c>
@@ -1928,6 +2292,9 @@
       <c r="C40">
         <v>1.33</v>
       </c>
+      <c r="D40">
+        <v>3.6</v>
+      </c>
       <c r="M40">
         <v>2.85</v>
       </c>
@@ -1937,14 +2304,20 @@
       <c r="AA40">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="41" spans="1:29">
+      <c r="AF40">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:35">
       <c r="B41" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C41">
         <v>0.96199999999999997</v>
       </c>
+      <c r="D41">
+        <v>2.6</v>
+      </c>
       <c r="E41" s="2">
         <v>3.4</v>
       </c>
@@ -1957,14 +2330,20 @@
       <c r="AA41">
         <v>3.05</v>
       </c>
-    </row>
-    <row r="42" spans="1:29">
+      <c r="AF41">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35">
       <c r="B42" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C42">
         <v>0.61499999999999999</v>
       </c>
+      <c r="D42">
+        <v>1.5</v>
+      </c>
       <c r="M42">
         <v>1.25</v>
       </c>
@@ -1974,14 +2353,20 @@
       <c r="AA42">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="43" spans="1:29">
+      <c r="AF42">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:35">
       <c r="B43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C43">
         <v>0.65600000000000003</v>
       </c>
+      <c r="D43">
+        <v>1.6</v>
+      </c>
       <c r="M43">
         <v>1.3</v>
       </c>
@@ -1991,8 +2376,11 @@
       <c r="AA43">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="44" spans="1:29">
+      <c r="AF43">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35">
       <c r="B44" s="3" t="s">
         <v>21</v>
       </c>
@@ -2038,8 +2426,14 @@
       <c r="AA44">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="45" spans="1:29">
+      <c r="AF44">
+        <v>15</v>
+      </c>
+      <c r="AG44">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:35">
       <c r="B45" s="3" t="s">
         <v>22</v>
       </c>
@@ -2085,8 +2479,14 @@
       <c r="AA45">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="46" spans="1:29">
+      <c r="AF45">
+        <v>3.3</v>
+      </c>
+      <c r="AG45">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35">
       <c r="B46" s="3" t="s">
         <v>23</v>
       </c>
@@ -2111,8 +2511,14 @@
       <c r="AA46">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:29">
+      <c r="AF46">
+        <v>1.8</v>
+      </c>
+      <c r="AG46">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:35">
       <c r="B47" s="3" t="s">
         <v>24</v>
       </c>
@@ -2137,8 +2543,14 @@
       <c r="AA47">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="48" spans="1:29">
+      <c r="AF47">
+        <v>0.76</v>
+      </c>
+      <c r="AG47">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35">
       <c r="B48" s="3" t="s">
         <v>25</v>
       </c>
@@ -2166,8 +2578,11 @@
       <c r="AC48">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:31">
+      <c r="AF48">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32">
       <c r="B49" s="3" t="s">
         <v>26</v>
       </c>
@@ -2183,8 +2598,11 @@
       <c r="AA49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:31">
+      <c r="AF49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32">
       <c r="B50" s="3" t="s">
         <v>27</v>
       </c>
@@ -2197,8 +2615,11 @@
       <c r="AA50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:31">
+      <c r="AF50">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32">
       <c r="B51" s="3" t="s">
         <v>38</v>
       </c>
@@ -2211,8 +2632,11 @@
       <c r="AA51">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:31">
+      <c r="AF51">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32">
       <c r="B52" s="3" t="s">
         <v>28</v>
       </c>
@@ -2243,8 +2667,11 @@
       <c r="AE52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:31">
+      <c r="AF52">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32">
       <c r="B53" s="3" t="s">
         <v>30</v>
       </c>
@@ -2263,8 +2690,11 @@
       <c r="AB53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:31">
+      <c r="AF53">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32">
       <c r="B54" s="3" t="s">
         <v>31</v>
       </c>
@@ -2298,8 +2728,11 @@
       <c r="AC54">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:31">
+      <c r="AF54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32">
       <c r="B55" s="3" t="s">
         <v>29</v>
       </c>
@@ -2318,46 +2751,99 @@
       <c r="AC55">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:31">
+      <c r="AF55">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32">
       <c r="A57" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57">
+        <v>8</v>
+      </c>
+      <c r="AF57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32">
+      <c r="B58" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="AF58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32">
+      <c r="B59" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59">
+        <v>8</v>
+      </c>
+      <c r="AF59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32">
+      <c r="B60" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+      <c r="AF60">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32">
+      <c r="A62" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C62" t="s">
         <v>36</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D62" t="s">
         <v>35</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F62" t="s">
         <v>43</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N62" t="s">
         <v>60</v>
       </c>
-      <c r="R57" t="s">
+      <c r="R62" t="s">
         <v>63</v>
       </c>
-      <c r="T57" t="s">
+      <c r="T62" t="s">
         <v>63</v>
       </c>
-      <c r="U57" t="s">
+      <c r="U62" t="s">
         <v>60</v>
       </c>
-      <c r="W57" t="s">
+      <c r="W62" t="s">
         <v>70</v>
       </c>
-      <c r="X57" s="5" t="s">
+      <c r="X62" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:31">
-      <c r="W58" t="s">
+      <c r="AF62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32">
+      <c r="W63" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:31">
-      <c r="W59" t="s">
+    <row r="64" spans="1:32">
+      <c r="W64" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add gap junctions; update analysis functions; continue tuning network parameters
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="234">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -640,6 +640,305 @@
   </si>
   <si>
     <t>long_noconn_49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constant_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time constant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduced from</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>400 to 150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constant_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constant_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">FSI2XX depression </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Increasing FSI drive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduces gamma power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Totally synchronized</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change shell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>firing rate</t>
+  </si>
+  <si>
+    <t>x 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>constant_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gap junction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSI2FSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTS2LTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_LTS_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_LTS_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>const_LTS_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_LTS_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_LTS_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_LTS_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_LTS_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_LTS_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_LTS_4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1044,10 +1343,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:BH72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="AT3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AX11" sqref="AX11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1056,15 +1358,180 @@
     <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.125" customWidth="1"/>
     <col min="4" max="4" width="9" style="11"/>
+    <col min="45" max="45" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:60">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O1" t="s">
+        <v>171</v>
+      </c>
+      <c r="P1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>179</v>
+      </c>
+      <c r="R1" t="s">
+        <v>172</v>
+      </c>
+      <c r="S1" t="s">
+        <v>178</v>
+      </c>
+      <c r="T1" t="s">
+        <v>180</v>
+      </c>
+      <c r="U1" t="s">
+        <v>173</v>
+      </c>
+      <c r="V1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>199</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>209</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>211</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>230</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>231</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>219</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>221</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>222</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>223</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>225</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>226</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>229</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>232</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1072,7 +1539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:60">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1082,68 +1549,1522 @@
       <c r="C3" s="12">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="E3">
+        <v>1.51</v>
+      </c>
+      <c r="F3">
+        <v>1.6</v>
+      </c>
+      <c r="G3">
+        <v>1.83</v>
+      </c>
+      <c r="H3">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="I3">
+        <v>1.88</v>
+      </c>
+      <c r="J3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K3">
+        <v>3.05</v>
+      </c>
+      <c r="L3">
+        <v>3.59</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="N3" s="7">
+        <v>2.12</v>
+      </c>
+      <c r="O3" s="7">
+        <v>1.88</v>
+      </c>
+      <c r="P3" s="7">
+        <v>3.12</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="R3" s="7">
+        <v>1.86</v>
+      </c>
+      <c r="S3" s="7">
+        <v>3.09</v>
+      </c>
+      <c r="T3" s="7">
+        <v>2.68</v>
+      </c>
+      <c r="U3" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="V3" s="7">
+        <v>1.95</v>
+      </c>
+      <c r="W3" s="7">
+        <v>2.42</v>
+      </c>
+      <c r="X3">
+        <v>1.54</v>
+      </c>
+      <c r="Y3">
+        <v>2.08</v>
+      </c>
+      <c r="Z3">
+        <v>2.02</v>
+      </c>
+      <c r="AA3">
+        <v>2.84</v>
+      </c>
+      <c r="AB3">
+        <v>3.01</v>
+      </c>
+      <c r="AC3">
+        <v>3.99</v>
+      </c>
+      <c r="AD3">
+        <v>2.73</v>
+      </c>
+      <c r="AE3">
+        <v>2.39</v>
+      </c>
+      <c r="AF3">
+        <v>3.14</v>
+      </c>
+      <c r="AG3">
+        <v>3.88</v>
+      </c>
+      <c r="AH3">
+        <v>3.15</v>
+      </c>
+      <c r="AI3">
+        <v>3.82</v>
+      </c>
+      <c r="AJ3">
+        <v>2.5</v>
+      </c>
+      <c r="AK3">
+        <v>3.21</v>
+      </c>
+      <c r="AL3">
+        <v>4.34</v>
+      </c>
+      <c r="AM3">
+        <v>2.08</v>
+      </c>
+      <c r="AN3">
+        <v>2.81</v>
+      </c>
+      <c r="AO3">
+        <v>3.1</v>
+      </c>
+      <c r="AP3">
+        <v>3.26</v>
+      </c>
+      <c r="AQ3">
+        <v>2.63</v>
+      </c>
+      <c r="AR3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AS3">
+        <v>1.88</v>
+      </c>
+      <c r="AT3">
+        <v>1.85</v>
+      </c>
+      <c r="AU3">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AV3">
+        <v>2.71</v>
+      </c>
+      <c r="AW3">
+        <v>2.15</v>
+      </c>
+      <c r="AX3">
+        <v>1.83</v>
+      </c>
+      <c r="AZ3">
+        <v>1.89</v>
+      </c>
+      <c r="BA3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BB3">
+        <v>3.22</v>
+      </c>
+      <c r="BC3">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="BD3">
+        <v>2.59</v>
+      </c>
+      <c r="BE3">
+        <v>2.29</v>
+      </c>
+      <c r="BF3">
+        <v>2.37</v>
+      </c>
+      <c r="BG3">
+        <v>2.06</v>
+      </c>
+      <c r="BH3">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="12">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="E4">
+        <v>1.42</v>
+      </c>
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>1.61</v>
+      </c>
+      <c r="H4">
+        <v>1.98</v>
+      </c>
+      <c r="I4">
+        <v>1.64</v>
+      </c>
+      <c r="J4">
+        <v>1.53</v>
+      </c>
+      <c r="K4">
+        <v>1.49</v>
+      </c>
+      <c r="L4">
+        <v>1.87</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1.43</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="P4" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="R4" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="S4" s="7">
+        <v>1.69</v>
+      </c>
+      <c r="T4" s="7">
+        <v>1.39</v>
+      </c>
+      <c r="U4" s="7">
+        <v>1.42</v>
+      </c>
+      <c r="V4" s="7">
+        <v>1.39</v>
+      </c>
+      <c r="W4" s="7">
+        <v>1.31</v>
+      </c>
+      <c r="X4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Y4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Z4">
+        <v>1.73</v>
+      </c>
+      <c r="AA4">
+        <v>1.89</v>
+      </c>
+      <c r="AB4">
+        <v>2.08</v>
+      </c>
+      <c r="AC4">
+        <v>2.14</v>
+      </c>
+      <c r="AD4">
+        <v>1.85</v>
+      </c>
+      <c r="AE4">
+        <v>1.71</v>
+      </c>
+      <c r="AF4">
+        <v>2.09</v>
+      </c>
+      <c r="AG4">
+        <v>2</v>
+      </c>
+      <c r="AH4">
+        <v>1.84</v>
+      </c>
+      <c r="AI4">
+        <v>1.88</v>
+      </c>
+      <c r="AJ4">
+        <v>1.66</v>
+      </c>
+      <c r="AK4">
+        <v>1.85</v>
+      </c>
+      <c r="AL4">
+        <v>1.94</v>
+      </c>
+      <c r="AM4">
+        <v>1.39</v>
+      </c>
+      <c r="AN4">
+        <v>1.5</v>
+      </c>
+      <c r="AO4">
+        <v>1.54</v>
+      </c>
+      <c r="AP4">
+        <v>1.85</v>
+      </c>
+      <c r="AQ4">
+        <v>1.55</v>
+      </c>
+      <c r="AR4">
+        <v>1.52</v>
+      </c>
+      <c r="AS4">
+        <v>1.68</v>
+      </c>
+      <c r="AT4">
+        <v>1.54</v>
+      </c>
+      <c r="AU4">
+        <v>1.57</v>
+      </c>
+      <c r="AV4">
+        <v>1.43</v>
+      </c>
+      <c r="AW4">
+        <v>1.75</v>
+      </c>
+      <c r="AX4">
+        <v>1.65</v>
+      </c>
+      <c r="AZ4">
+        <v>1.87</v>
+      </c>
+      <c r="BA4">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BB4">
+        <v>2.33</v>
+      </c>
+      <c r="BC4">
+        <v>1.68</v>
+      </c>
+      <c r="BD4">
+        <v>1.91</v>
+      </c>
+      <c r="BE4">
+        <v>2.13</v>
+      </c>
+      <c r="BF4">
+        <v>1.66</v>
+      </c>
+      <c r="BG4">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BH4">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="12">
         <v>0.84</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="E5">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="F5">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="G5">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="H5">
+        <v>1.32</v>
+      </c>
+      <c r="I5">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="J5">
+        <v>0.9</v>
+      </c>
+      <c r="K5">
+        <v>1.57</v>
+      </c>
+      <c r="L5">
+        <v>1.62</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="P5" s="7">
+        <v>1.66</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>1.61</v>
+      </c>
+      <c r="R5" s="7">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="S5" s="7">
+        <v>1.76</v>
+      </c>
+      <c r="T5" s="7">
+        <v>1.67</v>
+      </c>
+      <c r="U5" s="7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="V5" s="7">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="W5" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="X5">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="Y5">
+        <v>1.35</v>
+      </c>
+      <c r="Z5">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AA5">
+        <v>1.3</v>
+      </c>
+      <c r="AB5">
+        <v>1.38</v>
+      </c>
+      <c r="AC5">
+        <v>2.08</v>
+      </c>
+      <c r="AD5">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AE5">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="AF5">
+        <v>1.47</v>
+      </c>
+      <c r="AG5">
+        <v>2</v>
+      </c>
+      <c r="AH5">
+        <v>1.18</v>
+      </c>
+      <c r="AI5">
+        <v>1.62</v>
+      </c>
+      <c r="AJ5">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="AK5">
+        <v>1.92</v>
+      </c>
+      <c r="AL5">
+        <v>3.05</v>
+      </c>
+      <c r="AM5">
+        <v>1.37</v>
+      </c>
+      <c r="AN5">
+        <v>2.08</v>
+      </c>
+      <c r="AO5">
+        <v>2.33</v>
+      </c>
+      <c r="AP5">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AQ5">
+        <v>1.85</v>
+      </c>
+      <c r="AR5">
+        <v>1.78</v>
+      </c>
+      <c r="AS5">
+        <v>1.34</v>
+      </c>
+      <c r="AT5">
+        <v>1.34</v>
+      </c>
+      <c r="AU5">
+        <v>1.26</v>
+      </c>
+      <c r="AV5">
+        <v>1.98</v>
+      </c>
+      <c r="AW5">
+        <v>1.3</v>
+      </c>
+      <c r="AX5">
+        <v>1.4</v>
+      </c>
+      <c r="AZ5">
+        <v>1.18</v>
+      </c>
+      <c r="BA5">
+        <v>1.49</v>
+      </c>
+      <c r="BB5">
+        <v>3.33</v>
+      </c>
+      <c r="BC5">
+        <v>2.76</v>
+      </c>
+      <c r="BD5">
+        <v>2.85</v>
+      </c>
+      <c r="BE5">
+        <v>1.51</v>
+      </c>
+      <c r="BF5">
+        <v>2.69</v>
+      </c>
+      <c r="BG5">
+        <v>1.35</v>
+      </c>
+      <c r="BH5">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G6">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="H6">
+        <v>1.39</v>
+      </c>
+      <c r="I6">
+        <v>1.02</v>
+      </c>
+      <c r="J6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K6">
+        <v>1.18</v>
+      </c>
+      <c r="L6">
+        <v>1.59</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1.07</v>
+      </c>
+      <c r="P6" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="R6" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S6" s="7">
+        <v>1.57</v>
+      </c>
+      <c r="T6" s="7">
+        <v>1.17</v>
+      </c>
+      <c r="U6" s="7">
+        <v>1.02</v>
+      </c>
+      <c r="V6" s="7">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="W6" s="7">
+        <v>1.01</v>
+      </c>
+      <c r="X6">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="Y6">
+        <v>1.06</v>
+      </c>
+      <c r="Z6">
+        <v>1.04</v>
+      </c>
+      <c r="AA6">
+        <v>1.17</v>
+      </c>
+      <c r="AB6">
+        <v>1.4</v>
+      </c>
+      <c r="AC6">
+        <v>1.47</v>
+      </c>
+      <c r="AD6">
+        <v>1.22</v>
+      </c>
+      <c r="AE6">
+        <v>1.06</v>
+      </c>
+      <c r="AF6">
+        <v>1.44</v>
+      </c>
+      <c r="AG6">
+        <v>1.36</v>
+      </c>
+      <c r="AH6">
+        <v>1.25</v>
+      </c>
+      <c r="AI6">
+        <v>1.27</v>
+      </c>
+      <c r="AJ6">
+        <v>1.07</v>
+      </c>
+      <c r="AK6">
+        <v>1.77</v>
+      </c>
+      <c r="AL6">
+        <v>1.88</v>
+      </c>
+      <c r="AM6">
+        <v>1.4</v>
+      </c>
+      <c r="AN6">
+        <v>1.47</v>
+      </c>
+      <c r="AO6">
+        <v>1.46</v>
+      </c>
+      <c r="AP6">
+        <v>1.9</v>
+      </c>
+      <c r="AQ6">
+        <v>1.57</v>
+      </c>
+      <c r="AR6">
+        <v>1.53</v>
+      </c>
+      <c r="AS6">
+        <v>1.38</v>
+      </c>
+      <c r="AT6">
+        <v>1.37</v>
+      </c>
+      <c r="AU6">
+        <v>1.32</v>
+      </c>
+      <c r="AV6">
+        <v>1.31</v>
+      </c>
+      <c r="AW6">
+        <v>1.37</v>
+      </c>
+      <c r="AX6">
+        <v>1.44</v>
+      </c>
+      <c r="AZ6">
+        <v>1.27</v>
+      </c>
+      <c r="BA6">
+        <v>1.49</v>
+      </c>
+      <c r="BB6">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BC6">
+        <v>1.55</v>
+      </c>
+      <c r="BD6">
+        <v>1.65</v>
+      </c>
+      <c r="BE6">
+        <v>1.49</v>
+      </c>
+      <c r="BF6">
+        <v>1.56</v>
+      </c>
+      <c r="BG6">
+        <v>1.38</v>
+      </c>
+      <c r="BH6">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:60">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="12">
         <v>5.15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="E7">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="F7">
+        <v>6.15</v>
+      </c>
+      <c r="G7">
+        <v>8.31</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>7.09</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <v>24.8</v>
+      </c>
+      <c r="L7">
+        <v>32.6</v>
+      </c>
+      <c r="M7" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="N7" s="7">
+        <v>15.3</v>
+      </c>
+      <c r="O7" s="7">
+        <v>6.15</v>
+      </c>
+      <c r="P7" s="7">
+        <v>17.2</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>13.7</v>
+      </c>
+      <c r="R7" s="7">
+        <v>6.23</v>
+      </c>
+      <c r="S7" s="7">
+        <v>17.7</v>
+      </c>
+      <c r="T7" s="7">
+        <v>14</v>
+      </c>
+      <c r="U7" s="7">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="V7" s="7">
+        <v>6.32</v>
+      </c>
+      <c r="W7" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="X7">
+        <v>7.34</v>
+      </c>
+      <c r="Y7">
+        <v>11.4</v>
+      </c>
+      <c r="Z7">
+        <v>13.1</v>
+      </c>
+      <c r="AA7">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="AB7">
+        <v>5.16</v>
+      </c>
+      <c r="AC7">
+        <v>7.41</v>
+      </c>
+      <c r="AD7">
+        <v>7.36</v>
+      </c>
+      <c r="AE7">
+        <v>10.4</v>
+      </c>
+      <c r="AF7">
+        <v>5.49</v>
+      </c>
+      <c r="AG7">
+        <v>9.81</v>
+      </c>
+      <c r="AH7">
+        <v>5.22</v>
+      </c>
+      <c r="AI7">
+        <v>6.72</v>
+      </c>
+      <c r="AJ7">
+        <v>9.86</v>
+      </c>
+      <c r="AK7">
+        <v>6.02</v>
+      </c>
+      <c r="AL7">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="AM7">
+        <v>7.07</v>
+      </c>
+      <c r="AN7">
+        <v>10.4</v>
+      </c>
+      <c r="AO7">
+        <v>10.3</v>
+      </c>
+      <c r="AP7">
+        <v>11.9</v>
+      </c>
+      <c r="AQ7">
+        <v>23.6</v>
+      </c>
+      <c r="AR7">
+        <v>23.7</v>
+      </c>
+      <c r="AS7">
+        <v>2.84</v>
+      </c>
+      <c r="AT7">
+        <v>4.62</v>
+      </c>
+      <c r="AU7">
+        <v>6.05</v>
+      </c>
+      <c r="AV7">
+        <v>10.7</v>
+      </c>
+      <c r="AW7">
+        <v>12.6</v>
+      </c>
+      <c r="AX7">
+        <v>11</v>
+      </c>
+      <c r="AZ7">
+        <v>6.25</v>
+      </c>
+      <c r="BA7">
+        <v>7.65</v>
+      </c>
+      <c r="BB7">
+        <v>13.8</v>
+      </c>
+      <c r="BC7">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="BD7">
+        <v>12.5</v>
+      </c>
+      <c r="BE7">
+        <v>5.27</v>
+      </c>
+      <c r="BF7">
+        <v>6.16</v>
+      </c>
+      <c r="BG7">
+        <v>12.4</v>
+      </c>
+      <c r="BH7">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60">
       <c r="C8" s="12">
         <v>6.11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="11">
+        <v>6.4</v>
+      </c>
+      <c r="E8">
+        <v>7.15</v>
+      </c>
+      <c r="F8">
+        <v>4.58</v>
+      </c>
+      <c r="G8">
+        <v>5.24</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>4.84</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="L8">
+        <v>10.1</v>
+      </c>
+      <c r="M8" s="7">
+        <v>7.22</v>
+      </c>
+      <c r="N8" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="O8" s="7">
+        <v>4.42</v>
+      </c>
+      <c r="P8" s="7">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>8</v>
+      </c>
+      <c r="R8" s="7">
+        <v>4.46</v>
+      </c>
+      <c r="S8" s="7">
+        <v>9.74</v>
+      </c>
+      <c r="T8" s="7">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="U8" s="7">
+        <v>3.45</v>
+      </c>
+      <c r="V8" s="7">
+        <v>5.32</v>
+      </c>
+      <c r="W8" s="7">
+        <v>6.64</v>
+      </c>
+      <c r="X8">
+        <v>5.72</v>
+      </c>
+      <c r="Y8">
+        <v>7.9</v>
+      </c>
+      <c r="Z8">
+        <v>9.73</v>
+      </c>
+      <c r="AA8">
+        <v>13.4</v>
+      </c>
+      <c r="AB8">
+        <v>4.3</v>
+      </c>
+      <c r="AC8">
+        <v>5.86</v>
+      </c>
+      <c r="AD8">
+        <v>7.24</v>
+      </c>
+      <c r="AE8">
+        <v>5.52</v>
+      </c>
+      <c r="AF8">
+        <v>4.55</v>
+      </c>
+      <c r="AG8">
+        <v>6.42</v>
+      </c>
+      <c r="AH8">
+        <v>4.34</v>
+      </c>
+      <c r="AI8">
+        <v>5.33</v>
+      </c>
+      <c r="AJ8">
+        <v>7.06</v>
+      </c>
+      <c r="AK8">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="AL8">
+        <v>7.17</v>
+      </c>
+      <c r="AM8">
+        <v>5.51</v>
+      </c>
+      <c r="AN8">
+        <v>7.63</v>
+      </c>
+      <c r="AO8">
+        <v>7.57</v>
+      </c>
+      <c r="AP8">
+        <v>8.61</v>
+      </c>
+      <c r="AQ8">
+        <v>0.35</v>
+      </c>
+      <c r="AR8">
+        <v>1.52</v>
+      </c>
+      <c r="AS8">
+        <v>2.77</v>
+      </c>
+      <c r="AT8">
+        <v>3.27</v>
+      </c>
+      <c r="AU8">
+        <v>5.6</v>
+      </c>
+      <c r="AV8">
+        <v>6.39</v>
+      </c>
+      <c r="AW8">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="AX8">
+        <v>7.71</v>
+      </c>
+      <c r="AZ8">
+        <v>5.26</v>
+      </c>
+      <c r="BA8">
+        <v>6.16</v>
+      </c>
+      <c r="BB8">
+        <v>10.6</v>
+      </c>
+      <c r="BC8">
+        <v>7.09</v>
+      </c>
+      <c r="BD8">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="BE8">
+        <v>4.55</v>
+      </c>
+      <c r="BF8">
+        <v>5.03</v>
+      </c>
+      <c r="BG8">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="BH8">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="12">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="11">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1.39</v>
+      </c>
+      <c r="F9">
+        <v>1.36</v>
+      </c>
+      <c r="G9">
+        <v>1.24</v>
+      </c>
+      <c r="H9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I9">
+        <v>1.24</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="AF9">
+        <v>3.34</v>
+      </c>
+      <c r="AH9">
+        <v>3.34</v>
+      </c>
+      <c r="AQ9">
+        <v>1.37</v>
+      </c>
+      <c r="AR9">
+        <v>1.53</v>
+      </c>
+      <c r="AS9">
+        <v>2.52</v>
+      </c>
+      <c r="AV9">
+        <v>8.11</v>
+      </c>
+      <c r="AW9">
+        <v>9.25</v>
+      </c>
+      <c r="AX9">
+        <v>4.16</v>
+      </c>
+      <c r="AZ9">
+        <v>7.16</v>
+      </c>
+      <c r="BA9">
+        <v>4.84</v>
+      </c>
+      <c r="BB9">
+        <v>15.2</v>
+      </c>
+      <c r="BC9">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="BD9">
+        <v>13.1</v>
+      </c>
+      <c r="BE9">
+        <v>4.87</v>
+      </c>
+      <c r="BF9">
+        <v>19.2</v>
+      </c>
+      <c r="BG9">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="BH9">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:60">
       <c r="C10" s="12">
         <v>4.07</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="11">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>2.82</v>
+      </c>
+      <c r="F10">
+        <v>2.79</v>
+      </c>
+      <c r="G10">
+        <v>2.64</v>
+      </c>
+      <c r="H10">
+        <v>4.63</v>
+      </c>
+      <c r="I10">
+        <v>2.64</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="AF10">
+        <v>4.54</v>
+      </c>
+      <c r="AH10">
+        <v>4.54</v>
+      </c>
+      <c r="AQ10">
+        <v>3.17</v>
+      </c>
+      <c r="AR10">
+        <v>3.32</v>
+      </c>
+      <c r="AS10">
+        <v>4.07</v>
+      </c>
+      <c r="AV10">
+        <v>6.21</v>
+      </c>
+      <c r="AW10">
+        <v>6.5</v>
+      </c>
+      <c r="AX10">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="AZ10">
+        <v>5.16</v>
+      </c>
+      <c r="BA10">
+        <v>3.7</v>
+      </c>
+      <c r="BB10">
+        <v>6.43</v>
+      </c>
+      <c r="BC10">
+        <v>6.43</v>
+      </c>
+      <c r="BD10">
+        <v>5.67</v>
+      </c>
+      <c r="BE10">
+        <v>3.85</v>
+      </c>
+      <c r="BF10">
+        <v>6.53</v>
+      </c>
+      <c r="BG10">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="BH10">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:60">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="J11">
+        <v>25.1</v>
+      </c>
+      <c r="K11">
+        <v>31.1</v>
+      </c>
+      <c r="L11">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="N11" s="7">
+        <v>33</v>
+      </c>
+      <c r="O11" s="7">
+        <v>29.7</v>
+      </c>
+      <c r="P11" s="7">
+        <v>35.4</v>
+      </c>
+      <c r="Q11">
+        <v>30.4</v>
+      </c>
+      <c r="R11">
+        <v>30</v>
+      </c>
+      <c r="S11">
+        <v>37.5</v>
+      </c>
+      <c r="T11">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="U11">
+        <v>26.6</v>
+      </c>
+      <c r="V11">
+        <v>30.1</v>
+      </c>
+      <c r="W11" s="7">
+        <v>35.5</v>
+      </c>
+      <c r="X11" s="7">
+        <v>31.5</v>
+      </c>
+      <c r="Y11" s="7">
+        <v>36.6</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>42.2</v>
+      </c>
+      <c r="AA11">
+        <v>48.2</v>
+      </c>
+      <c r="AB11">
+        <v>32.9</v>
+      </c>
+      <c r="AC11">
+        <v>38</v>
+      </c>
+      <c r="AD11">
+        <v>38.5</v>
+      </c>
+      <c r="AE11">
+        <v>27.4</v>
+      </c>
+      <c r="AF11">
+        <v>28.2</v>
+      </c>
+      <c r="AG11">
+        <v>30.7</v>
+      </c>
+      <c r="AH11">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="AI11">
+        <v>36.6</v>
+      </c>
+      <c r="AJ11">
+        <v>34</v>
+      </c>
+      <c r="AK11">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="AL11">
+        <v>41.7</v>
+      </c>
+      <c r="AM11">
+        <v>33.5</v>
+      </c>
+      <c r="AN11">
+        <v>39.1</v>
+      </c>
+      <c r="AO11">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="AP11">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="AQ11">
+        <v>23.8</v>
+      </c>
+      <c r="AR11">
+        <v>24.1</v>
+      </c>
+      <c r="AS11">
+        <v>26.6</v>
+      </c>
+      <c r="AT11">
+        <v>28.5</v>
+      </c>
+      <c r="AU11">
+        <v>33.9</v>
+      </c>
+      <c r="AV11">
+        <v>36.1</v>
+      </c>
+      <c r="BB11">
+        <v>26.7</v>
+      </c>
+      <c r="BD11">
+        <v>19.8</v>
+      </c>
+      <c r="BF11">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="J12">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K12">
+        <v>1.2</v>
+      </c>
+      <c r="L12">
+        <v>1.08</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0.66</v>
+      </c>
+      <c r="Q12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R12">
+        <v>0.4</v>
+      </c>
+      <c r="S12">
+        <v>1.57</v>
+      </c>
+      <c r="T12">
+        <v>1.28</v>
+      </c>
+      <c r="U12">
+        <v>0.33</v>
+      </c>
+      <c r="V12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="W12" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="X12" s="7">
+        <v>0.62</v>
+      </c>
+      <c r="Y12" s="7">
+        <v>1.17</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AA12">
+        <v>1.64</v>
+      </c>
+      <c r="AB12">
+        <v>1.22</v>
+      </c>
+      <c r="AC12">
+        <v>1.76</v>
+      </c>
+      <c r="AD12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AE12">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="AF12">
+        <v>1.8</v>
+      </c>
+      <c r="AG12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AH12">
+        <v>1.32</v>
+      </c>
+      <c r="AI12">
+        <v>1.68</v>
+      </c>
+      <c r="AJ12">
+        <v>1.8</v>
+      </c>
+      <c r="AK12">
+        <v>0.49</v>
+      </c>
+      <c r="AL12">
+        <v>0.77</v>
+      </c>
+      <c r="AM12">
+        <v>1.39</v>
+      </c>
+      <c r="AN12">
+        <v>1.76</v>
+      </c>
+      <c r="AO12">
+        <v>1.95</v>
+      </c>
+      <c r="AP12">
+        <v>2.29</v>
+      </c>
+      <c r="AQ12">
+        <v>2.31</v>
+      </c>
+      <c r="AR12">
+        <v>2.04</v>
+      </c>
+      <c r="AS12">
+        <v>1.32</v>
+      </c>
+      <c r="AT12">
+        <v>1.72</v>
+      </c>
+      <c r="AU12">
+        <v>1.21</v>
+      </c>
+      <c r="AV12">
+        <v>2.14</v>
+      </c>
+      <c r="BB12">
+        <v>0.53</v>
+      </c>
+      <c r="BD12">
+        <v>0.62</v>
+      </c>
+      <c r="BF12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:60">
+      <c r="AE13">
+        <v>55.8</v>
+      </c>
+      <c r="AF13">
+        <v>55.7</v>
+      </c>
+      <c r="AG13">
+        <v>61</v>
+      </c>
+      <c r="AO13">
+        <v>76</v>
+      </c>
+      <c r="AP13">
+        <v>76.7</v>
+      </c>
+      <c r="AQ13">
+        <v>47.4</v>
+      </c>
+      <c r="AR13">
+        <v>48.2</v>
+      </c>
+      <c r="AT13">
+        <v>56.5</v>
+      </c>
+      <c r="AV13">
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:60">
+      <c r="AE14">
+        <v>1.7</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>1.65</v>
+      </c>
+      <c r="AO14">
+        <v>0.75</v>
+      </c>
+      <c r="AP14">
+        <v>1.34</v>
+      </c>
+      <c r="AQ14">
+        <v>1.79</v>
+      </c>
+      <c r="AR14">
+        <v>2.02</v>
+      </c>
+      <c r="AT14">
+        <v>1.17</v>
+      </c>
+      <c r="AV14">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:59">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1153,37 +3074,208 @@
       <c r="D17" s="11">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>8</v>
+      </c>
+      <c r="N17">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <v>8.5</v>
+      </c>
+      <c r="V17">
+        <v>8.5</v>
+      </c>
+      <c r="X17">
+        <v>10</v>
+      </c>
+      <c r="Z17">
+        <v>19</v>
+      </c>
+      <c r="AH17">
+        <v>14.5</v>
+      </c>
+      <c r="AK17">
+        <v>14</v>
+      </c>
+      <c r="AM17">
+        <v>13</v>
+      </c>
+      <c r="AS17">
+        <v>7.5</v>
+      </c>
+      <c r="AT17">
+        <v>8</v>
+      </c>
+      <c r="AU17">
+        <v>8.5</v>
+      </c>
+      <c r="AW17">
+        <v>8</v>
+      </c>
+      <c r="AX17">
+        <v>7.5</v>
+      </c>
+      <c r="AZ17">
+        <v>7.5</v>
+      </c>
+      <c r="BG17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:59">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="G18">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>10.5</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>13</v>
+      </c>
+      <c r="M18">
+        <v>11</v>
+      </c>
+      <c r="N18">
+        <v>13</v>
+      </c>
+      <c r="O18">
+        <v>12</v>
+      </c>
+      <c r="V18">
+        <v>12.5</v>
+      </c>
+      <c r="X18">
+        <v>14</v>
+      </c>
+      <c r="Z18">
+        <v>20</v>
+      </c>
+      <c r="AH18">
+        <v>18</v>
+      </c>
+      <c r="AK18">
+        <v>18</v>
+      </c>
+      <c r="AM18">
+        <v>20</v>
+      </c>
+      <c r="AS18">
+        <v>13</v>
+      </c>
+      <c r="AT18">
+        <v>14</v>
+      </c>
+      <c r="AU18">
+        <v>14.5</v>
+      </c>
+      <c r="AW18">
+        <v>14</v>
+      </c>
+      <c r="AZ18">
+        <v>10</v>
+      </c>
+      <c r="BA18">
+        <v>10.5</v>
+      </c>
+      <c r="BG18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:59">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>0.5</v>
+      </c>
+      <c r="H19">
+        <v>0.2</v>
+      </c>
+      <c r="I19">
+        <v>0.5</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>3</v>
+      </c>
+      <c r="AE19">
+        <v>0.5</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AU19">
+        <v>2</v>
+      </c>
+      <c r="AW19">
+        <v>1</v>
+      </c>
+      <c r="AZ19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="AF20">
+        <v>1.5</v>
+      </c>
+      <c r="AW20">
+        <v>2</v>
+      </c>
+      <c r="AX20">
+        <v>1</v>
+      </c>
+      <c r="AZ20">
+        <v>1</v>
+      </c>
+      <c r="BA20">
+        <v>0.5</v>
+      </c>
+      <c r="BG20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59">
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:59">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -1196,8 +3288,20 @@
       <c r="D22" s="11">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:59">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -1207,8 +3311,20 @@
       <c r="D23" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK23" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:59">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1218,8 +3334,20 @@
       <c r="D24" s="11">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:59">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1229,8 +3357,20 @@
       <c r="D25" s="11">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH25" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK25" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:59">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -1240,8 +3380,53 @@
       <c r="D26" s="11">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" t="s">
+        <v>161</v>
+      </c>
+      <c r="M26">
+        <v>7.2</v>
+      </c>
+      <c r="O26">
+        <v>5.4</v>
+      </c>
+      <c r="X26">
+        <v>7.2</v>
+      </c>
+      <c r="Z26">
+        <v>13.5</v>
+      </c>
+      <c r="AB26">
+        <v>5.4</v>
+      </c>
+      <c r="AJ26">
+        <v>7.2</v>
+      </c>
+      <c r="AK26">
+        <v>5.4</v>
+      </c>
+      <c r="AM26">
+        <v>7.2</v>
+      </c>
+      <c r="AS26">
+        <v>6.3</v>
+      </c>
+      <c r="AT26">
+        <v>7.2</v>
+      </c>
+      <c r="AW26" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="AZ26">
+        <v>7.2</v>
+      </c>
+      <c r="BG26" s="11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:59">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -1251,8 +3436,53 @@
       <c r="D27" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="H27" t="s">
+        <v>160</v>
+      </c>
+      <c r="I27" t="s">
+        <v>161</v>
+      </c>
+      <c r="M27">
+        <v>1.6</v>
+      </c>
+      <c r="O27">
+        <v>1.2</v>
+      </c>
+      <c r="X27">
+        <v>1.6</v>
+      </c>
+      <c r="Z27">
+        <v>3</v>
+      </c>
+      <c r="AB27">
+        <v>1.2</v>
+      </c>
+      <c r="AJ27">
+        <v>1.6</v>
+      </c>
+      <c r="AK27">
+        <v>1.2</v>
+      </c>
+      <c r="AM27">
+        <v>1.6</v>
+      </c>
+      <c r="AS27">
+        <v>1.4</v>
+      </c>
+      <c r="AT27">
+        <v>1.6</v>
+      </c>
+      <c r="AW27" s="11">
+        <v>1.65</v>
+      </c>
+      <c r="AZ27">
+        <v>1.6</v>
+      </c>
+      <c r="BG27" s="11">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:59">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -1262,8 +3492,32 @@
       <c r="D28" s="11">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>160</v>
+      </c>
+      <c r="H28" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV28">
+        <v>0.93</v>
+      </c>
+      <c r="AW28" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="AZ28">
+        <v>0.84</v>
+      </c>
+      <c r="BA28">
+        <v>0.93</v>
+      </c>
+      <c r="BG28" s="11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:59">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -1273,8 +3527,32 @@
       <c r="D29" s="11">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV29">
+        <v>0.39</v>
+      </c>
+      <c r="AW29" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="AZ29">
+        <v>0.35</v>
+      </c>
+      <c r="BA29">
+        <v>0.39</v>
+      </c>
+      <c r="BG29" s="11">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:59">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -1284,8 +3562,59 @@
       <c r="D30" s="11">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="H30" t="s">
+        <v>160</v>
+      </c>
+      <c r="I30" t="s">
+        <v>161</v>
+      </c>
+      <c r="J30">
+        <v>3.6</v>
+      </c>
+      <c r="M30">
+        <v>2.4</v>
+      </c>
+      <c r="N30">
+        <v>3.6</v>
+      </c>
+      <c r="R30">
+        <v>6.1</v>
+      </c>
+      <c r="U30">
+        <v>3.6</v>
+      </c>
+      <c r="X30">
+        <v>4.8</v>
+      </c>
+      <c r="Z30">
+        <v>7.2</v>
+      </c>
+      <c r="AB30">
+        <v>9.6</v>
+      </c>
+      <c r="AJ30">
+        <v>7.2</v>
+      </c>
+      <c r="AK30">
+        <v>4.8</v>
+      </c>
+      <c r="AM30">
+        <v>7.2</v>
+      </c>
+      <c r="AS30">
+        <v>4.8</v>
+      </c>
+      <c r="AW30" s="11">
+        <v>2.4</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>212</v>
+      </c>
+      <c r="BG30" s="11">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:59">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -1295,8 +3624,59 @@
       <c r="D31" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="H31" t="s">
+        <v>160</v>
+      </c>
+      <c r="I31" t="s">
+        <v>161</v>
+      </c>
+      <c r="J31">
+        <v>4.5</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>4.5</v>
+      </c>
+      <c r="R31">
+        <v>7.6</v>
+      </c>
+      <c r="U31">
+        <v>4.5</v>
+      </c>
+      <c r="X31">
+        <v>6</v>
+      </c>
+      <c r="Z31">
+        <v>9</v>
+      </c>
+      <c r="AB31">
+        <v>12</v>
+      </c>
+      <c r="AJ31">
+        <v>9</v>
+      </c>
+      <c r="AK31">
+        <v>6</v>
+      </c>
+      <c r="AM31">
+        <v>9</v>
+      </c>
+      <c r="AS31">
+        <v>6</v>
+      </c>
+      <c r="AW31" s="11">
+        <v>3</v>
+      </c>
+      <c r="AZ31" t="s">
+        <v>212</v>
+      </c>
+      <c r="BG31" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:59">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -1306,8 +3686,26 @@
       <c r="D32" s="11">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" t="s">
+        <v>161</v>
+      </c>
+      <c r="I32" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW32" s="11">
+        <v>1</v>
+      </c>
+      <c r="AZ32">
+        <v>1.7</v>
+      </c>
+      <c r="BG32" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:59">
       <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
@@ -1317,8 +3715,26 @@
       <c r="D33" s="11">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW33" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="AZ33">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BG33" s="11">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:59">
       <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
@@ -1328,8 +3744,53 @@
       <c r="D34" s="11">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="F34">
+        <v>1.5</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1.5</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="M34">
+        <v>9</v>
+      </c>
+      <c r="X34">
+        <v>12</v>
+      </c>
+      <c r="Z34">
+        <v>30</v>
+      </c>
+      <c r="AE34">
+        <v>6</v>
+      </c>
+      <c r="AH34">
+        <v>30</v>
+      </c>
+      <c r="AJ34">
+        <v>15</v>
+      </c>
+      <c r="AK34">
+        <v>30</v>
+      </c>
+      <c r="AM34">
+        <v>20</v>
+      </c>
+      <c r="AW34" s="7">
+        <v>10</v>
+      </c>
+      <c r="AZ34">
+        <v>20</v>
+      </c>
+      <c r="BG34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:59">
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
@@ -1339,8 +3800,12 @@
       <c r="D35" s="11">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW35" s="7"/>
+    </row>
+    <row r="36" spans="1:59">
       <c r="B36" s="3" t="s">
         <v>31</v>
       </c>
@@ -1350,8 +3815,18 @@
       <c r="D36" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF36">
+        <v>3</v>
+      </c>
+      <c r="AH36" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW36" s="7"/>
+    </row>
+    <row r="37" spans="1:59">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -1361,177 +3836,287 @@
       <c r="D37" s="11">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0.5</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="AW37" s="7">
+        <v>3</v>
+      </c>
+      <c r="BG37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:59">
       <c r="C38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="AW38" s="7"/>
+    </row>
+    <row r="39" spans="1:59">
       <c r="A39" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" s="11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>217</v>
+      </c>
+      <c r="AQ39" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR39">
+        <v>3.3E-4</v>
+      </c>
+      <c r="AS39">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="AW39">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="AZ39" t="s">
+        <v>227</v>
+      </c>
+      <c r="BE39">
+        <v>6.6000000000000005E-5</v>
+      </c>
+      <c r="BG39">
+        <v>2.1999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:59">
+      <c r="B40" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D40" s="11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>217</v>
+      </c>
+      <c r="AQ40" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR40">
+        <v>3.8000000000000002E-4</v>
+      </c>
+      <c r="AS40">
+        <v>7.6000000000000004E-5</v>
+      </c>
+      <c r="AW40">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="AZ40" t="s">
+        <v>227</v>
+      </c>
+      <c r="BE40">
+        <v>7.6000000000000004E-5</v>
+      </c>
+      <c r="BG40">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:59">
+      <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D42" s="11">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40" s="3" t="s">
+      <c r="R42">
+        <v>4</v>
+      </c>
+      <c r="U42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:59">
+      <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D43" s="11">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="B41" s="3" t="s">
+    <row r="44" spans="1:59">
+      <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D44" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="B42" s="3" t="s">
+    <row r="45" spans="1:59">
+      <c r="B45" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D45" s="11">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="3" t="s">
+    <row r="46" spans="1:59">
+      <c r="A46" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D46" s="11">
         <v>2.9</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="B44" s="3" t="s">
+    <row r="47" spans="1:59">
+      <c r="B47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D47" s="11">
         <v>3.8</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="B45" s="3" t="s">
+    <row r="48" spans="1:59">
+      <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D48" s="11">
         <v>3.9</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="B46" s="3" t="s">
+    <row r="49" spans="1:39">
+      <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D49" s="11">
         <v>7.5</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="3" t="s">
+    <row r="51" spans="1:39">
+      <c r="A51" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
+      <c r="U51" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>192</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM51" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:39">
+      <c r="U52" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>193</v>
+      </c>
+      <c r="AM52" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:39">
+      <c r="U53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:39">
+      <c r="U54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39">
+      <c r="A56" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
+    <row r="57" spans="1:39">
+      <c r="A57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="D54" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D57" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="B58" s="3" t="s">
-        <v>5</v>
+    <row r="58" spans="1:39">
+      <c r="A58" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D58" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:39">
+      <c r="A59" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D59" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:39">
+      <c r="A60" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="D60" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:39">
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D61" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
-      <c r="B62" s="3" t="s">
-        <v>6</v>
-      </c>
+    <row r="62" spans="1:39">
       <c r="D62" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:39">
       <c r="D63" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:39">
       <c r="D64" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="2:4">
+      <c r="B65" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D65" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:4">
-      <c r="B66" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="D66" s="11">
         <v>0</v>
       </c>
@@ -1547,7 +4132,25 @@
       </c>
     </row>
     <row r="69" spans="2:4">
+      <c r="B69" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="D69" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="D70" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="D71" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="D72" s="11">
         <v>0</v>
       </c>
     </row>
@@ -1563,10 +4166,10 @@
   <dimension ref="A1:CE69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AE33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
+      <selection pane="bottomRight" activeCell="AF50" sqref="AF50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
Add network without STP
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="382">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1514,6 +1514,22 @@
   </si>
   <si>
     <t>long_r13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r13_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exc syn no STP as well</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r13_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r13_no_STP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1918,13 +1934,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN59"/>
+  <dimension ref="A1:AQ59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI11" sqref="AI11"/>
+      <selection pane="bottomRight" activeCell="AP20" sqref="AP20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1947,7 +1963,7 @@
     <col min="39" max="40" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:43">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2054,8 +2070,17 @@
       <c r="AN1" s="9" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="2" spans="1:40">
+      <c r="AO1" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2066,7 +2091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:43">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2184,8 +2209,17 @@
       <c r="AN3" s="9">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:40">
+      <c r="AO3">
+        <v>1.77</v>
+      </c>
+      <c r="AP3">
+        <v>2.46</v>
+      </c>
+      <c r="AQ3">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2297,8 +2331,17 @@
       <c r="AN4" s="9">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:40">
+      <c r="AO4">
+        <v>1.51</v>
+      </c>
+      <c r="AP4">
+        <v>1.41</v>
+      </c>
+      <c r="AQ4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2413,8 +2456,17 @@
       <c r="AN5" s="9">
         <v>2.69</v>
       </c>
-    </row>
-    <row r="6" spans="1:40">
+      <c r="AO5">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="AP5">
+        <v>1.29</v>
+      </c>
+      <c r="AQ5">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -2523,8 +2575,17 @@
       <c r="AN6" s="9">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="7" spans="1:40">
+      <c r="AO6">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2639,8 +2700,17 @@
       <c r="AN7" s="9">
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:40">
+      <c r="AO7">
+        <v>6.41</v>
+      </c>
+      <c r="AP7">
+        <v>10.8</v>
+      </c>
+      <c r="AQ7">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -2749,8 +2819,17 @@
       <c r="AN8" s="9">
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:40">
+      <c r="AO8">
+        <v>5.66</v>
+      </c>
+      <c r="AP8">
+        <v>7.76</v>
+      </c>
+      <c r="AQ8">
+        <v>8.0399999999999991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -2865,8 +2944,17 @@
       <c r="AN9" s="9">
         <v>13.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:40">
+      <c r="AO9">
+        <v>2.15</v>
+      </c>
+      <c r="AP9">
+        <v>1.77</v>
+      </c>
+      <c r="AQ9">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -2975,8 +3063,17 @@
       <c r="AN10" s="9">
         <v>6.96</v>
       </c>
-    </row>
-    <row r="11" spans="1:40">
+      <c r="AO10">
+        <v>6.78</v>
+      </c>
+      <c r="AP10">
+        <v>4.8</v>
+      </c>
+      <c r="AQ10">
+        <v>6.34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -3046,8 +3143,17 @@
       <c r="AN11" s="9">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:40">
+      <c r="AO11">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="AP11">
+        <v>38.6</v>
+      </c>
+      <c r="AQ11">
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -3114,8 +3220,17 @@
       <c r="AN12" s="9">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="13" spans="1:40">
+      <c r="AO12">
+        <v>0.6</v>
+      </c>
+      <c r="AP12">
+        <v>1.62</v>
+      </c>
+      <c r="AQ12">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -3140,8 +3255,14 @@
       <c r="AN13" s="9">
         <v>36.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:40">
+      <c r="AP13">
+        <v>76.7</v>
+      </c>
+      <c r="AQ13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -3165,6 +3286,12 @@
       </c>
       <c r="AN14" s="9">
         <v>0.44</v>
+      </c>
+      <c r="AP14">
+        <v>0.77</v>
+      </c>
+      <c r="AQ14">
+        <v>0.92</v>
       </c>
     </row>
     <row r="17" spans="1:38">
@@ -3844,7 +3971,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:41">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -3855,7 +3982,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:41">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -3869,7 +3996,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:41">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -3882,8 +4009,11 @@
       <c r="AL52" s="5">
         <v>400</v>
       </c>
-    </row>
-    <row r="53" spans="1:38">
+      <c r="AO52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -3893,8 +4023,11 @@
       <c r="AL53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:38">
+      <c r="AO53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -3905,15 +4038,18 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:41">
       <c r="D55" s="11">
         <v>25</v>
       </c>
       <c r="AL55" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:38">
+      <c r="AO55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:41">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -3923,16 +4059,22 @@
       <c r="AL56" s="5">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:38">
+      <c r="AO56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:41">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
       <c r="L58" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="59" spans="1:38">
+      <c r="AO58" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="59" spans="1:41">
       <c r="L59" t="s">
         <v>350</v>
       </c>

</xml_diff>

<commit_message>
Tuned model for correct gap juction connectivity
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="413">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1530,6 +1530,130 @@
   </si>
   <si>
     <t>long_r13_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Correct gap junction connectivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r33_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r33_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r33_no_STP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1934,13 +2058,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ59"/>
+  <dimension ref="A1:BW59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AP20" sqref="AP20"/>
+      <selection pane="bottomRight" activeCell="AR10" sqref="AR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1961,9 +2085,13 @@
     <col min="31" max="32" width="9" style="7"/>
     <col min="38" max="38" width="9" style="5"/>
     <col min="39" max="40" width="9" style="9"/>
+    <col min="44" max="44" width="9" style="7"/>
+    <col min="52" max="52" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="9" style="5"/>
+    <col min="71" max="72" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:75">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2079,8 +2207,95 @@
       <c r="AQ1" s="7" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="2" spans="1:43">
+      <c r="AR1" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="AW1" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="AX1" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="AY1" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="BA1" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="BB1" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="BC1" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="BE1" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="BF1" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="BG1" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="BI1" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="BJ1" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="BK1" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="BN1" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="BS1" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="BT1" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="BU1" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="BV1" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="BW1" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:75">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2091,7 +2306,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:75">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2218,8 +2433,104 @@
       <c r="AQ3">
         <v>2.46</v>
       </c>
-    </row>
-    <row r="4" spans="1:43">
+      <c r="AR3" s="7">
+        <v>1.87</v>
+      </c>
+      <c r="AS3" s="7">
+        <v>1.87</v>
+      </c>
+      <c r="AT3" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="AU3" s="7">
+        <v>1.89</v>
+      </c>
+      <c r="AV3" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="AW3" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="AX3" s="7">
+        <v>2.91</v>
+      </c>
+      <c r="AY3" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="AZ3">
+        <v>2.9</v>
+      </c>
+      <c r="BA3">
+        <v>2.14</v>
+      </c>
+      <c r="BB3">
+        <v>1.92</v>
+      </c>
+      <c r="BC3">
+        <v>2.88</v>
+      </c>
+      <c r="BD3">
+        <v>2.04</v>
+      </c>
+      <c r="BE3">
+        <v>1.93</v>
+      </c>
+      <c r="BF3">
+        <v>1.92</v>
+      </c>
+      <c r="BG3">
+        <v>1.91</v>
+      </c>
+      <c r="BH3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="BI3">
+        <v>1.94</v>
+      </c>
+      <c r="BJ3">
+        <v>1.89</v>
+      </c>
+      <c r="BK3">
+        <v>1.89</v>
+      </c>
+      <c r="BL3">
+        <v>1.87</v>
+      </c>
+      <c r="BM3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="BN3">
+        <v>1.89</v>
+      </c>
+      <c r="BO3">
+        <v>1.9</v>
+      </c>
+      <c r="BP3">
+        <v>1.9</v>
+      </c>
+      <c r="BQ3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="BR3" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="BS3" s="9">
+        <v>2.87</v>
+      </c>
+      <c r="BT3" s="9">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BU3">
+        <v>1.76</v>
+      </c>
+      <c r="BV3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="BW3">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:75">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2340,8 +2651,104 @@
       <c r="AQ4">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="5" spans="1:43">
+      <c r="AR4" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="AS4" s="7">
+        <v>1.76</v>
+      </c>
+      <c r="AT4" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="AU4" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="AV4" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="AW4" s="7">
+        <v>1.77</v>
+      </c>
+      <c r="AX4" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="AY4" s="7">
+        <v>1.55</v>
+      </c>
+      <c r="AZ4">
+        <v>1.8</v>
+      </c>
+      <c r="BA4">
+        <v>1.52</v>
+      </c>
+      <c r="BB4">
+        <v>1.8</v>
+      </c>
+      <c r="BC4">
+        <v>1.79</v>
+      </c>
+      <c r="BD4">
+        <v>1.47</v>
+      </c>
+      <c r="BE4">
+        <v>1.79</v>
+      </c>
+      <c r="BF4">
+        <v>1.79</v>
+      </c>
+      <c r="BG4">
+        <v>1.8</v>
+      </c>
+      <c r="BH4" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="BI4">
+        <v>1.83</v>
+      </c>
+      <c r="BJ4">
+        <v>1.81</v>
+      </c>
+      <c r="BK4">
+        <v>1.81</v>
+      </c>
+      <c r="BL4">
+        <v>1.8</v>
+      </c>
+      <c r="BM4" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="BN4">
+        <v>1.78</v>
+      </c>
+      <c r="BO4">
+        <v>1.78</v>
+      </c>
+      <c r="BP4">
+        <v>1.78</v>
+      </c>
+      <c r="BQ4" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="BR4" s="5">
+        <v>1.76</v>
+      </c>
+      <c r="BS4" s="9">
+        <v>1.78</v>
+      </c>
+      <c r="BT4" s="9">
+        <v>1.47</v>
+      </c>
+      <c r="BU4">
+        <v>1.49</v>
+      </c>
+      <c r="BV4">
+        <v>1.38</v>
+      </c>
+      <c r="BW4">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:75">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2465,8 +2872,104 @@
       <c r="AQ5">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="6" spans="1:43">
+      <c r="AR5" s="7">
+        <v>1.23</v>
+      </c>
+      <c r="AS5" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="AT5" s="7">
+        <v>1.26</v>
+      </c>
+      <c r="AU5" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="AV5" s="7">
+        <v>1.27</v>
+      </c>
+      <c r="AW5" s="7">
+        <v>1.28</v>
+      </c>
+      <c r="AX5" s="7">
+        <v>2.16</v>
+      </c>
+      <c r="AY5" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="AZ5">
+        <v>2.19</v>
+      </c>
+      <c r="BA5">
+        <v>2.74</v>
+      </c>
+      <c r="BB5">
+        <v>1.34</v>
+      </c>
+      <c r="BC5">
+        <v>2.21</v>
+      </c>
+      <c r="BD5">
+        <v>2.74</v>
+      </c>
+      <c r="BE5">
+        <v>1.29</v>
+      </c>
+      <c r="BF5">
+        <v>1.3</v>
+      </c>
+      <c r="BG5">
+        <v>1.29</v>
+      </c>
+      <c r="BH5" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="BI5">
+        <v>1.28</v>
+      </c>
+      <c r="BJ5">
+        <v>1.32</v>
+      </c>
+      <c r="BK5">
+        <v>1.3</v>
+      </c>
+      <c r="BL5">
+        <v>1.3</v>
+      </c>
+      <c r="BM5" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="BN5">
+        <v>1.3</v>
+      </c>
+      <c r="BO5">
+        <v>1.3</v>
+      </c>
+      <c r="BP5">
+        <v>1.3</v>
+      </c>
+      <c r="BQ5" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="BR5" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="BS5" s="9">
+        <v>2.16</v>
+      </c>
+      <c r="BT5" s="9">
+        <v>2.7</v>
+      </c>
+      <c r="BU5">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="BV5">
+        <v>1.29</v>
+      </c>
+      <c r="BW5">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:75">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -2584,8 +3087,104 @@
       <c r="AQ6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:43">
+      <c r="AR6" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="AS6" s="7">
+        <v>1.32</v>
+      </c>
+      <c r="AT6" s="7">
+        <v>1.32</v>
+      </c>
+      <c r="AU6" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="AV6" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="AW6" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="AX6" s="7">
+        <v>1.43</v>
+      </c>
+      <c r="AY6" s="7">
+        <v>1.59</v>
+      </c>
+      <c r="AZ6">
+        <v>1.44</v>
+      </c>
+      <c r="BA6">
+        <v>1.62</v>
+      </c>
+      <c r="BB6">
+        <v>1.38</v>
+      </c>
+      <c r="BC6">
+        <v>1.45</v>
+      </c>
+      <c r="BD6">
+        <v>1.63</v>
+      </c>
+      <c r="BE6">
+        <v>1.34</v>
+      </c>
+      <c r="BF6">
+        <v>1.34</v>
+      </c>
+      <c r="BG6">
+        <v>1.36</v>
+      </c>
+      <c r="BH6" s="12">
+        <v>1.35</v>
+      </c>
+      <c r="BI6">
+        <v>1.35</v>
+      </c>
+      <c r="BJ6">
+        <v>1.37</v>
+      </c>
+      <c r="BK6">
+        <v>1.36</v>
+      </c>
+      <c r="BL6">
+        <v>1.36</v>
+      </c>
+      <c r="BM6" s="12">
+        <v>1.35</v>
+      </c>
+      <c r="BN6">
+        <v>1.37</v>
+      </c>
+      <c r="BO6">
+        <v>1.36</v>
+      </c>
+      <c r="BP6">
+        <v>1.36</v>
+      </c>
+      <c r="BQ6" s="12">
+        <v>1.35</v>
+      </c>
+      <c r="BR6" s="5">
+        <v>1.35</v>
+      </c>
+      <c r="BS6" s="9">
+        <v>1.43</v>
+      </c>
+      <c r="BT6" s="9">
+        <v>1.6</v>
+      </c>
+      <c r="BU6">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="BV6">
+        <v>0.99</v>
+      </c>
+      <c r="BW6">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:75">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2709,8 +3308,104 @@
       <c r="AQ7">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:43">
+      <c r="AR7" s="7">
+        <v>8.43</v>
+      </c>
+      <c r="AS7" s="7">
+        <v>7.84</v>
+      </c>
+      <c r="AT7" s="7">
+        <v>7.84</v>
+      </c>
+      <c r="AU7" s="7">
+        <v>7.67</v>
+      </c>
+      <c r="AV7" s="7">
+        <v>7.59</v>
+      </c>
+      <c r="AW7" s="7">
+        <v>7.47</v>
+      </c>
+      <c r="AX7" s="7">
+        <v>17.8</v>
+      </c>
+      <c r="AY7" s="7">
+        <v>6.28</v>
+      </c>
+      <c r="AZ7">
+        <v>16.7</v>
+      </c>
+      <c r="BA7">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="BB7">
+        <v>6.58</v>
+      </c>
+      <c r="BC7">
+        <v>16.2</v>
+      </c>
+      <c r="BD7">
+        <v>4.26</v>
+      </c>
+      <c r="BE7">
+        <v>7.73</v>
+      </c>
+      <c r="BF7">
+        <v>7.5</v>
+      </c>
+      <c r="BG7">
+        <v>7.53</v>
+      </c>
+      <c r="BH7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="BI7">
+        <v>7.87</v>
+      </c>
+      <c r="BJ7">
+        <v>7.22</v>
+      </c>
+      <c r="BK7">
+        <v>7.49</v>
+      </c>
+      <c r="BL7">
+        <v>7.37</v>
+      </c>
+      <c r="BM7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="BN7">
+        <v>7.54</v>
+      </c>
+      <c r="BO7">
+        <v>7.57</v>
+      </c>
+      <c r="BP7">
+        <v>7.48</v>
+      </c>
+      <c r="BQ7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="BR7" s="5">
+        <v>7.47</v>
+      </c>
+      <c r="BS7" s="9">
+        <v>17.5</v>
+      </c>
+      <c r="BT7" s="9">
+        <v>5.14</v>
+      </c>
+      <c r="BU7">
+        <v>6.39</v>
+      </c>
+      <c r="BV7">
+        <v>10.7</v>
+      </c>
+      <c r="BW7">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:75">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -2828,8 +3523,104 @@
       <c r="AQ8">
         <v>8.0399999999999991</v>
       </c>
-    </row>
-    <row r="9" spans="1:43">
+      <c r="AR8" s="7">
+        <v>7.21</v>
+      </c>
+      <c r="AS8" s="7">
+        <v>6.77</v>
+      </c>
+      <c r="AT8" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="AU8" s="7">
+        <v>6.58</v>
+      </c>
+      <c r="AV8" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="AW8" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="AX8" s="7">
+        <v>11.4</v>
+      </c>
+      <c r="AY8" s="7">
+        <v>5.63</v>
+      </c>
+      <c r="AZ8">
+        <v>10.9</v>
+      </c>
+      <c r="BA8">
+        <v>4.79</v>
+      </c>
+      <c r="BB8">
+        <v>5.97</v>
+      </c>
+      <c r="BC8">
+        <v>10.7</v>
+      </c>
+      <c r="BD8">
+        <v>4.21</v>
+      </c>
+      <c r="BE8">
+        <v>6.83</v>
+      </c>
+      <c r="BF8">
+        <v>6.67</v>
+      </c>
+      <c r="BG8">
+        <v>6.66</v>
+      </c>
+      <c r="BH8" s="12">
+        <v>6.65</v>
+      </c>
+      <c r="BI8">
+        <v>6.9</v>
+      </c>
+      <c r="BJ8">
+        <v>6.5</v>
+      </c>
+      <c r="BK8">
+        <v>6.7</v>
+      </c>
+      <c r="BL8">
+        <v>6.67</v>
+      </c>
+      <c r="BM8" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="BN8">
+        <v>6.72</v>
+      </c>
+      <c r="BO8">
+        <v>6.71</v>
+      </c>
+      <c r="BP8">
+        <v>6.65</v>
+      </c>
+      <c r="BQ8" s="12">
+        <v>6.7</v>
+      </c>
+      <c r="BR8" s="5">
+        <v>6.69</v>
+      </c>
+      <c r="BS8" s="9">
+        <v>11.3</v>
+      </c>
+      <c r="BT8" s="9">
+        <v>5.12</v>
+      </c>
+      <c r="BU8">
+        <v>5.57</v>
+      </c>
+      <c r="BV8">
+        <v>7.69</v>
+      </c>
+      <c r="BW8">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -2953,8 +3744,104 @@
       <c r="AQ9">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="10" spans="1:43">
+      <c r="AR9" s="7">
+        <v>4.96</v>
+      </c>
+      <c r="AS9" s="7">
+        <v>5.05</v>
+      </c>
+      <c r="AT9" s="7">
+        <v>4.97</v>
+      </c>
+      <c r="AU9" s="7">
+        <v>5.03</v>
+      </c>
+      <c r="AV9" s="7">
+        <v>5.01</v>
+      </c>
+      <c r="AW9" s="7">
+        <v>5</v>
+      </c>
+      <c r="AX9" s="7">
+        <v>6.48</v>
+      </c>
+      <c r="AY9" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="AZ9">
+        <v>6.65</v>
+      </c>
+      <c r="BA9">
+        <v>12.4</v>
+      </c>
+      <c r="BB9">
+        <v>5.16</v>
+      </c>
+      <c r="BC9">
+        <v>6.74</v>
+      </c>
+      <c r="BD9">
+        <v>13.1</v>
+      </c>
+      <c r="BE9">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="BF9">
+        <v>4.96</v>
+      </c>
+      <c r="BG9">
+        <v>4.99</v>
+      </c>
+      <c r="BH9" s="12">
+        <v>5</v>
+      </c>
+      <c r="BI9">
+        <v>4.83</v>
+      </c>
+      <c r="BJ9">
+        <v>4.92</v>
+      </c>
+      <c r="BK9">
+        <v>4.92</v>
+      </c>
+      <c r="BL9">
+        <v>4.99</v>
+      </c>
+      <c r="BM9" s="12">
+        <v>5</v>
+      </c>
+      <c r="BN9">
+        <v>5.01</v>
+      </c>
+      <c r="BO9">
+        <v>4.99</v>
+      </c>
+      <c r="BP9">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="BQ9" s="12">
+        <v>5</v>
+      </c>
+      <c r="BR9" s="5">
+        <v>5</v>
+      </c>
+      <c r="BS9" s="9">
+        <v>6.58</v>
+      </c>
+      <c r="BT9" s="9">
+        <v>12.7</v>
+      </c>
+      <c r="BU9">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BV9">
+        <v>1.74</v>
+      </c>
+      <c r="BW9">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -3072,8 +3959,104 @@
       <c r="AQ10">
         <v>6.34</v>
       </c>
-    </row>
-    <row r="11" spans="1:43">
+      <c r="AR10" s="7">
+        <v>5.82</v>
+      </c>
+      <c r="AS10" s="7">
+        <v>5.85</v>
+      </c>
+      <c r="AT10" s="7">
+        <v>5.8</v>
+      </c>
+      <c r="AU10" s="7">
+        <v>5.83</v>
+      </c>
+      <c r="AV10" s="7">
+        <v>5.81</v>
+      </c>
+      <c r="AW10" s="7">
+        <v>5.8</v>
+      </c>
+      <c r="AX10" s="7">
+        <v>6.23</v>
+      </c>
+      <c r="AY10" s="7">
+        <v>7.08</v>
+      </c>
+      <c r="AZ10">
+        <v>6.25</v>
+      </c>
+      <c r="BA10">
+        <v>7.15</v>
+      </c>
+      <c r="BB10">
+        <v>5.9</v>
+      </c>
+      <c r="BC10">
+        <v>6.28</v>
+      </c>
+      <c r="BD10">
+        <v>7.18</v>
+      </c>
+      <c r="BE10">
+        <v>5.82</v>
+      </c>
+      <c r="BF10">
+        <v>5.83</v>
+      </c>
+      <c r="BG10">
+        <v>5.85</v>
+      </c>
+      <c r="BH10" s="12">
+        <v>5.85</v>
+      </c>
+      <c r="BI10">
+        <v>5.8</v>
+      </c>
+      <c r="BJ10">
+        <v>5.85</v>
+      </c>
+      <c r="BK10">
+        <v>5.84</v>
+      </c>
+      <c r="BL10">
+        <v>5.89</v>
+      </c>
+      <c r="BM10" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="BN10">
+        <v>5.9</v>
+      </c>
+      <c r="BO10">
+        <v>5.87</v>
+      </c>
+      <c r="BP10">
+        <v>5.87</v>
+      </c>
+      <c r="BQ10" s="12">
+        <v>5.85</v>
+      </c>
+      <c r="BR10" s="5">
+        <v>5.85</v>
+      </c>
+      <c r="BS10" s="9">
+        <v>6.22</v>
+      </c>
+      <c r="BT10" s="9">
+        <v>7.11</v>
+      </c>
+      <c r="BU10">
+        <v>3.09</v>
+      </c>
+      <c r="BV10">
+        <v>3.58</v>
+      </c>
+      <c r="BW10">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:75">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -3152,8 +4135,29 @@
       <c r="AQ11">
         <v>39.299999999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:43">
+      <c r="AX11" s="7">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="AZ11">
+        <v>37.6</v>
+      </c>
+      <c r="BA11">
+        <v>21.2</v>
+      </c>
+      <c r="BC11">
+        <v>37.4</v>
+      </c>
+      <c r="BD11">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="BS11" s="9">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="BT11" s="9">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:75">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -3229,8 +4233,29 @@
       <c r="AQ12">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="13" spans="1:43">
+      <c r="AX12" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="AZ12">
+        <v>0.48</v>
+      </c>
+      <c r="BA12">
+        <v>0.38</v>
+      </c>
+      <c r="BC12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="BD12">
+        <v>0.53</v>
+      </c>
+      <c r="BS12" s="9">
+        <v>0.49</v>
+      </c>
+      <c r="BT12" s="9">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:75">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -3261,8 +4286,17 @@
       <c r="AQ13">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:43">
+      <c r="AY13">
+        <v>22</v>
+      </c>
+      <c r="BD13">
+        <v>37.6</v>
+      </c>
+      <c r="BT13" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:75">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -3293,8 +4327,17 @@
       <c r="AQ14">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="17" spans="1:38">
+      <c r="AY14" t="s">
+        <v>391</v>
+      </c>
+      <c r="BD14">
+        <v>0.48</v>
+      </c>
+      <c r="BT14" s="9">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -3343,8 +4386,32 @@
       <c r="AL17" s="5">
         <v>8.1300000000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:38">
+      <c r="BF17">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="BG17">
+        <v>8.11</v>
+      </c>
+      <c r="BJ17">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="BK17">
+        <v>8.06</v>
+      </c>
+      <c r="BL17">
+        <v>8.07</v>
+      </c>
+      <c r="BN17">
+        <v>8.11</v>
+      </c>
+      <c r="BO17">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="BR17" s="5">
+        <v>8.1300000000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -3378,8 +4445,11 @@
       <c r="AL18" s="5">
         <v>12.76</v>
       </c>
-    </row>
-    <row r="19" spans="1:38">
+      <c r="BR18" s="5">
+        <v>12.76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:70">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -3413,8 +4483,56 @@
       <c r="AL19" s="5">
         <v>1.6719999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:38">
+      <c r="AS19" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AT19">
+        <v>1.42</v>
+      </c>
+      <c r="AU19">
+        <v>1.4</v>
+      </c>
+      <c r="AV19">
+        <v>1.35</v>
+      </c>
+      <c r="AW19">
+        <v>1.3</v>
+      </c>
+      <c r="BE19">
+        <v>1.6</v>
+      </c>
+      <c r="BF19">
+        <v>1.55</v>
+      </c>
+      <c r="BG19">
+        <v>1.6</v>
+      </c>
+      <c r="BI19">
+        <v>1.59</v>
+      </c>
+      <c r="BJ19">
+        <v>1.5</v>
+      </c>
+      <c r="BK19">
+        <v>1.58</v>
+      </c>
+      <c r="BL19">
+        <v>1.6</v>
+      </c>
+      <c r="BN19">
+        <v>1.64</v>
+      </c>
+      <c r="BO19">
+        <v>1.62</v>
+      </c>
+      <c r="BP19">
+        <v>1.6</v>
+      </c>
+      <c r="BR19" s="5">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:70">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -3448,13 +4566,46 @@
       <c r="AL20" s="5">
         <v>2.23</v>
       </c>
-    </row>
-    <row r="21" spans="1:38">
+      <c r="AT20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AU20">
+        <v>2.21</v>
+      </c>
+      <c r="AV20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AW20">
+        <v>2.19</v>
+      </c>
+      <c r="BG20">
+        <v>2.21</v>
+      </c>
+      <c r="BJ20">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BK20">
+        <v>2.23</v>
+      </c>
+      <c r="BL20">
+        <v>2.25</v>
+      </c>
+      <c r="BN20">
+        <v>2.25</v>
+      </c>
+      <c r="BO20">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="BR20" s="5">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:70">
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:70">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -3477,7 +4628,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:70">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -3497,7 +4648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:70">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -3517,7 +4668,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:70">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -3537,7 +4688,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:70">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -3564,7 +4715,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:70">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -3591,7 +4742,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:70">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -3612,7 +4763,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:70">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -3633,7 +4784,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:70">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -3651,7 +4802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:70">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -3669,7 +4820,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:70">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -3690,7 +4841,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:57">
       <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
@@ -3711,7 +4862,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:57">
       <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
@@ -3744,7 +4895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:57">
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
@@ -3777,7 +4928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:57">
       <c r="B36" s="3" t="s">
         <v>31</v>
       </c>
@@ -3807,7 +4958,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:57">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -3834,12 +4985,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:57">
       <c r="C38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:57">
       <c r="A39" s="3" t="s">
         <v>213</v>
       </c>
@@ -3864,8 +5015,14 @@
       <c r="AL39" s="5">
         <v>3.3000000000000003E-5</v>
       </c>
-    </row>
-    <row r="40" spans="1:38">
+      <c r="AZ39">
+        <v>5.5000000000000002E-5</v>
+      </c>
+      <c r="BB39">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:57">
       <c r="B40" s="3" t="s">
         <v>215</v>
       </c>
@@ -3881,8 +5038,17 @@
       <c r="AL40" s="5">
         <v>3.8000000000000002E-4</v>
       </c>
-    </row>
-    <row r="42" spans="1:38">
+      <c r="AZ40">
+        <v>6.4999999999999997E-4</v>
+      </c>
+      <c r="BB40">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="BE40">
+        <v>6.8999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:57">
       <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
@@ -3896,7 +5062,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:57">
       <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
@@ -3910,7 +5076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:57">
       <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
@@ -3921,7 +5087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:57">
       <c r="B45" s="3" t="s">
         <v>85</v>
       </c>
@@ -3935,7 +5101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:57">
       <c r="A46" s="3" t="s">
         <v>82</v>
       </c>
@@ -3949,7 +5115,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:57">
       <c r="B47" s="3" t="s">
         <v>22</v>
       </c>
@@ -3960,7 +5126,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:57">
       <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
@@ -3971,7 +5137,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="49" spans="1:41">
+    <row r="49" spans="1:73">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -3982,7 +5148,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="51" spans="1:41">
+    <row r="51" spans="1:73">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -3996,7 +5162,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:41">
+    <row r="52" spans="1:73">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -4012,8 +5178,14 @@
       <c r="AO52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:41">
+      <c r="AR52" s="7">
+        <v>400</v>
+      </c>
+      <c r="BU52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:73">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -4026,8 +5198,14 @@
       <c r="AO53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:41">
+      <c r="AR53" s="7">
+        <v>0</v>
+      </c>
+      <c r="BU53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:73">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -4038,7 +5216,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:41">
+    <row r="55" spans="1:73">
       <c r="D55" s="11">
         <v>25</v>
       </c>
@@ -4048,8 +5226,14 @@
       <c r="AO55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:41">
+      <c r="AR55" s="7">
+        <v>25</v>
+      </c>
+      <c r="BU55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:73">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -4062,8 +5246,14 @@
       <c r="AO56">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:41">
+      <c r="AR56" s="7">
+        <v>200</v>
+      </c>
+      <c r="BU56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:73">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -4073,8 +5263,11 @@
       <c r="AO58" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="59" spans="1:41">
+      <c r="AR58" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="59" spans="1:73">
       <c r="L59" t="s">
         <v>350</v>
       </c>
@@ -4091,7 +5284,7 @@
   <dimension ref="A1:ES66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="EG3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="EO7" sqref="EO7"/>
@@ -10364,7 +11557,7 @@
   <dimension ref="A1:CE69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AZ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="K27" sqref="K27"/>

</xml_diff>

<commit_message>
Update analysis functions; Update a set of network parameters
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="427">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1654,6 +1654,62 @@
   </si>
   <si>
     <t>long_r33_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r41</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r43</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2058,13 +2114,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BW59"/>
+  <dimension ref="A1:CM59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CA9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AR10" sqref="AR10"/>
+      <selection pane="bottomRight" activeCell="CM21" sqref="CM21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2089,9 +2145,13 @@
     <col min="52" max="52" width="9.5" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="9" style="5"/>
     <col min="71" max="72" width="9" style="9"/>
+    <col min="76" max="76" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="87" max="88" width="9" style="7"/>
+    <col min="90" max="90" width="9" style="5"/>
+    <col min="91" max="91" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75">
+    <row r="1" spans="1:91">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2294,8 +2354,50 @@
       <c r="BW1" s="7" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="2" spans="1:75">
+      <c r="BX1" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="BY1" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="BZ1" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="CA1" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="CD1" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="CE1" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="CF1" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="CH1" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="CI1" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="CJ1" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="CK1" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="CL1" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="CM1" s="7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:91">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2306,7 +2408,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:75">
+    <row r="3" spans="1:91">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2529,8 +2631,53 @@
       <c r="BW3">
         <v>2.4500000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:75">
+      <c r="BX3">
+        <v>1.94</v>
+      </c>
+      <c r="BY3">
+        <v>1.93</v>
+      </c>
+      <c r="BZ3">
+        <v>1.92</v>
+      </c>
+      <c r="CA3">
+        <v>2.88</v>
+      </c>
+      <c r="CB3">
+        <v>2.09</v>
+      </c>
+      <c r="CC3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="CD3">
+        <v>1.9</v>
+      </c>
+      <c r="CE3">
+        <v>1.9</v>
+      </c>
+      <c r="CF3">
+        <v>1.9</v>
+      </c>
+      <c r="CG3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="CH3">
+        <v>1.9</v>
+      </c>
+      <c r="CI3" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="CJ3" s="7">
+        <v>2.87</v>
+      </c>
+      <c r="CK3">
+        <v>2.08</v>
+      </c>
+      <c r="CL3" s="5">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:91">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2747,8 +2894,53 @@
       <c r="BW4">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="5" spans="1:75">
+      <c r="BX4">
+        <v>1.79</v>
+      </c>
+      <c r="BY4">
+        <v>1.8</v>
+      </c>
+      <c r="BZ4">
+        <v>1.8</v>
+      </c>
+      <c r="CA4">
+        <v>1.77</v>
+      </c>
+      <c r="CB4">
+        <v>1.52</v>
+      </c>
+      <c r="CC4" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="CD4">
+        <v>1.79</v>
+      </c>
+      <c r="CE4">
+        <v>1.79</v>
+      </c>
+      <c r="CF4">
+        <v>1.79</v>
+      </c>
+      <c r="CG4" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="CH4">
+        <v>1.79</v>
+      </c>
+      <c r="CI4" s="7">
+        <v>1.79</v>
+      </c>
+      <c r="CJ4" s="7">
+        <v>1.81</v>
+      </c>
+      <c r="CK4">
+        <v>1.5</v>
+      </c>
+      <c r="CL4" s="5">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:91">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2968,8 +3160,53 @@
       <c r="BW5">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="6" spans="1:75">
+      <c r="BX5">
+        <v>1.2</v>
+      </c>
+      <c r="BY5">
+        <v>1.26</v>
+      </c>
+      <c r="BZ5">
+        <v>1.28</v>
+      </c>
+      <c r="CA5">
+        <v>2.12</v>
+      </c>
+      <c r="CB5">
+        <v>2.69</v>
+      </c>
+      <c r="CC5" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="CD5">
+        <v>1.28</v>
+      </c>
+      <c r="CE5">
+        <v>1.28</v>
+      </c>
+      <c r="CF5">
+        <v>1.3</v>
+      </c>
+      <c r="CG5" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="CH5">
+        <v>1.29</v>
+      </c>
+      <c r="CI5" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="CJ5" s="7">
+        <v>2.14</v>
+      </c>
+      <c r="CK5">
+        <v>2.73</v>
+      </c>
+      <c r="CL5" s="5">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:91">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3183,8 +3420,53 @@
       <c r="BW6">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="7" spans="1:75">
+      <c r="BX6">
+        <v>1.3</v>
+      </c>
+      <c r="BY6">
+        <v>1.34</v>
+      </c>
+      <c r="BZ6">
+        <v>1.36</v>
+      </c>
+      <c r="CA6">
+        <v>1.42</v>
+      </c>
+      <c r="CB6">
+        <v>1.64</v>
+      </c>
+      <c r="CC6" s="12">
+        <v>1.35</v>
+      </c>
+      <c r="CD6">
+        <v>1.37</v>
+      </c>
+      <c r="CE6">
+        <v>1.36</v>
+      </c>
+      <c r="CF6">
+        <v>1.38</v>
+      </c>
+      <c r="CG6" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="CH6">
+        <v>1.37</v>
+      </c>
+      <c r="CI6" s="7">
+        <v>1.37</v>
+      </c>
+      <c r="CJ6" s="7">
+        <v>1.47</v>
+      </c>
+      <c r="CK6">
+        <v>1.67</v>
+      </c>
+      <c r="CL6" s="5">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:91">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3404,8 +3686,53 @@
       <c r="BW7">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:75">
+      <c r="BX7">
+        <v>9.24</v>
+      </c>
+      <c r="BY7">
+        <v>7.83</v>
+      </c>
+      <c r="BZ7">
+        <v>7.38</v>
+      </c>
+      <c r="CA7">
+        <v>18.3</v>
+      </c>
+      <c r="CB7">
+        <v>5.37</v>
+      </c>
+      <c r="CC7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="CD7">
+        <v>7.19</v>
+      </c>
+      <c r="CE7">
+        <v>7.47</v>
+      </c>
+      <c r="CF7">
+        <v>7.48</v>
+      </c>
+      <c r="CG7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="CH7">
+        <v>7.48</v>
+      </c>
+      <c r="CI7" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="CJ7" s="7">
+        <v>18.7</v>
+      </c>
+      <c r="CK7">
+        <v>5.5</v>
+      </c>
+      <c r="CL7" s="5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:91">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -3619,8 +3946,53 @@
       <c r="BW8">
         <v>7.85</v>
       </c>
-    </row>
-    <row r="9" spans="1:75">
+      <c r="BX8">
+        <v>7.19</v>
+      </c>
+      <c r="BY8">
+        <v>6.19</v>
+      </c>
+      <c r="BZ8">
+        <v>5.91</v>
+      </c>
+      <c r="CA8">
+        <v>11.2</v>
+      </c>
+      <c r="CB8">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="CC8" s="12">
+        <v>6</v>
+      </c>
+      <c r="CD8">
+        <v>5.76</v>
+      </c>
+      <c r="CE8">
+        <v>5.96</v>
+      </c>
+      <c r="CF8">
+        <v>5.98</v>
+      </c>
+      <c r="CG8" s="12">
+        <v>6</v>
+      </c>
+      <c r="CH8">
+        <v>5.99</v>
+      </c>
+      <c r="CI8" s="7">
+        <v>6.02</v>
+      </c>
+      <c r="CJ8" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="CK8">
+        <v>4.74</v>
+      </c>
+      <c r="CL8" s="5">
+        <v>6.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:91">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -3840,8 +4212,53 @@
       <c r="BW9">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="10" spans="1:75">
+      <c r="BX9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="BY9">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="BZ9">
+        <v>4.95</v>
+      </c>
+      <c r="CA9">
+        <v>6.41</v>
+      </c>
+      <c r="CB9">
+        <v>12.6</v>
+      </c>
+      <c r="CC9" s="12">
+        <v>5</v>
+      </c>
+      <c r="CD9">
+        <v>4.96</v>
+      </c>
+      <c r="CE9">
+        <v>4.92</v>
+      </c>
+      <c r="CF9">
+        <v>4.97</v>
+      </c>
+      <c r="CG9" s="12">
+        <v>5</v>
+      </c>
+      <c r="CH9">
+        <v>5</v>
+      </c>
+      <c r="CI9" s="7">
+        <v>5</v>
+      </c>
+      <c r="CJ9" s="7">
+        <v>6.43</v>
+      </c>
+      <c r="CK9">
+        <v>12.6</v>
+      </c>
+      <c r="CL9" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:91">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -4055,8 +4472,53 @@
       <c r="BW10">
         <v>3.54</v>
       </c>
-    </row>
-    <row r="11" spans="1:75">
+      <c r="BX10">
+        <v>5.73</v>
+      </c>
+      <c r="BY10">
+        <v>5.81</v>
+      </c>
+      <c r="BZ10">
+        <v>5.87</v>
+      </c>
+      <c r="CA10">
+        <v>6.18</v>
+      </c>
+      <c r="CB10">
+        <v>7.2</v>
+      </c>
+      <c r="CC10" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="CD10">
+        <v>5.92</v>
+      </c>
+      <c r="CE10">
+        <v>5.9</v>
+      </c>
+      <c r="CF10">
+        <v>5.92</v>
+      </c>
+      <c r="CG10" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="CH10">
+        <v>5.94</v>
+      </c>
+      <c r="CI10" s="7">
+        <v>5.93</v>
+      </c>
+      <c r="CJ10" s="7">
+        <v>6.36</v>
+      </c>
+      <c r="CK10">
+        <v>7.23</v>
+      </c>
+      <c r="CL10" s="5">
+        <v>5.93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:91">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -4156,8 +4618,17 @@
       <c r="BT11" s="9">
         <v>18.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:75">
+      <c r="CA11">
+        <v>37.5</v>
+      </c>
+      <c r="CB11">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="CJ11" s="7">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:91">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -4254,8 +4725,17 @@
       <c r="BT12" s="9">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="13" spans="1:75">
+      <c r="CA12">
+        <v>0.47</v>
+      </c>
+      <c r="CB12">
+        <v>0.4</v>
+      </c>
+      <c r="CJ12" s="7">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:91">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -4295,8 +4775,11 @@
       <c r="BT13" s="9">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:75">
+      <c r="CB13">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:91">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -4336,8 +4819,11 @@
       <c r="BT14" s="9">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="17" spans="1:70">
+      <c r="CB14">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:91">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -4410,8 +4896,20 @@
       <c r="BR17" s="5">
         <v>8.1300000000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:70">
+      <c r="CD17">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="CF17">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="CI17">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="CL17" s="5">
+        <v>8.1300000000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:91">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -4448,8 +4946,26 @@
       <c r="BR18" s="5">
         <v>12.76</v>
       </c>
-    </row>
-    <row r="19" spans="1:70">
+      <c r="CD18">
+        <v>12.78</v>
+      </c>
+      <c r="CE18">
+        <v>12.8</v>
+      </c>
+      <c r="CF18">
+        <v>12.87</v>
+      </c>
+      <c r="CH18">
+        <v>12.88</v>
+      </c>
+      <c r="CI18" s="7">
+        <v>12.89</v>
+      </c>
+      <c r="CL18" s="5">
+        <v>12.91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:91">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -4531,8 +5047,38 @@
       <c r="BR19" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:70">
+      <c r="BX19">
+        <v>1.2</v>
+      </c>
+      <c r="BY19">
+        <v>0.8</v>
+      </c>
+      <c r="BZ19">
+        <v>0.7</v>
+      </c>
+      <c r="CD19">
+        <v>0.71</v>
+      </c>
+      <c r="CE19">
+        <v>0.78</v>
+      </c>
+      <c r="CF19">
+        <v>0.79</v>
+      </c>
+      <c r="CH19">
+        <v>0.81</v>
+      </c>
+      <c r="CI19" s="7">
+        <v>0.82</v>
+      </c>
+      <c r="CL19" s="5">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="CM19">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:91">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -4599,13 +5145,28 @@
       <c r="BR20" s="5">
         <v>2.23</v>
       </c>
-    </row>
-    <row r="21" spans="1:70">
+      <c r="CF20">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="CH20">
+        <v>2.25</v>
+      </c>
+      <c r="CI20" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="CL20" s="5">
+        <v>2.25</v>
+      </c>
+      <c r="CM20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:91">
       <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:70">
+    <row r="22" spans="1:91">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -4627,8 +5188,11 @@
       <c r="AL22" s="5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:70">
+      <c r="BR22" s="5">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:91">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -4647,8 +5211,11 @@
       <c r="AL23" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:70">
+      <c r="BR23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:91">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -4667,8 +5234,11 @@
       <c r="AL24" s="5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:70">
+      <c r="BR24" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:91">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -4687,8 +5257,11 @@
       <c r="AL25" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:70">
+      <c r="BR25" s="5">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:91">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -4714,8 +5287,20 @@
       <c r="AL26" s="5">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:70">
+      <c r="BR26" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="BX26">
+        <v>9</v>
+      </c>
+      <c r="CL26" s="5">
+        <v>9</v>
+      </c>
+      <c r="CM26">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:91">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -4741,8 +5326,20 @@
       <c r="AL27" s="5">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="28" spans="1:70">
+      <c r="BR27" s="5">
+        <v>1.88</v>
+      </c>
+      <c r="BX27">
+        <v>2</v>
+      </c>
+      <c r="CL27" s="5">
+        <v>2</v>
+      </c>
+      <c r="CM27">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:91">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -4762,8 +5359,14 @@
       <c r="AL28" s="5">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="29" spans="1:70">
+      <c r="BR28" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="CM28">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:91">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -4783,8 +5386,14 @@
       <c r="AL29" s="5">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="30" spans="1:70">
+      <c r="BR29" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="CM29">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:91">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -4801,8 +5410,11 @@
       <c r="AL30" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:70">
+      <c r="BR30" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:91">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -4819,8 +5431,11 @@
       <c r="AL31" s="5">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="32" spans="1:70">
+      <c r="BR31" s="5">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:91">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -4840,8 +5455,11 @@
       <c r="AL32" s="5">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="33" spans="1:57">
+      <c r="BR32" s="5">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:91">
       <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
@@ -4861,8 +5479,11 @@
       <c r="AL33" s="5">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:57">
+      <c r="BR33" s="5">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:91">
       <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
@@ -4894,8 +5515,11 @@
       <c r="AL34" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:57">
+      <c r="BR34" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:91">
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
@@ -4927,8 +5551,11 @@
       <c r="AL35" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:57">
+      <c r="BR35" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:91">
       <c r="B36" s="3" t="s">
         <v>31</v>
       </c>
@@ -4957,8 +5584,11 @@
       <c r="AL36" s="5">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:57">
+      <c r="BR36" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:91">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -4984,13 +5614,16 @@
       <c r="AL37" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:57">
+      <c r="BR37" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:91">
       <c r="C38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:57">
+    <row r="39" spans="1:91">
       <c r="A39" s="3" t="s">
         <v>213</v>
       </c>
@@ -5021,8 +5654,23 @@
       <c r="BB39">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="40" spans="1:57">
+      <c r="BR39" s="5">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="BX39">
+        <v>3.3000000000000003E-5</v>
+      </c>
+      <c r="CI39" s="7">
+        <v>3.3000000000000003E-5</v>
+      </c>
+      <c r="CL39" s="5">
+        <v>3.3000000000000003E-5</v>
+      </c>
+      <c r="CM39">
+        <v>6.6000000000000005E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:91">
       <c r="B40" s="3" t="s">
         <v>215</v>
       </c>
@@ -5047,8 +5695,20 @@
       <c r="BE40">
         <v>6.8999999999999997E-4</v>
       </c>
-    </row>
-    <row r="42" spans="1:57">
+      <c r="BR40" s="5">
+        <v>6.8999999999999997E-4</v>
+      </c>
+      <c r="CI40" s="7">
+        <v>6.8999999999999997E-4</v>
+      </c>
+      <c r="CL40" s="5">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="CM40">
+        <v>3.8000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:91">
       <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
@@ -5061,8 +5721,11 @@
       <c r="AL42" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:57">
+      <c r="BR42" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:91">
       <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
@@ -5075,8 +5738,11 @@
       <c r="AL43" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:57">
+      <c r="BR43" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:91">
       <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
@@ -5086,8 +5752,11 @@
       <c r="AL44" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:57">
+      <c r="BR44" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:91">
       <c r="B45" s="3" t="s">
         <v>85</v>
       </c>
@@ -5100,8 +5769,11 @@
       <c r="AL45" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:57">
+      <c r="BR45" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:91">
       <c r="A46" s="3" t="s">
         <v>82</v>
       </c>
@@ -5114,8 +5786,11 @@
       <c r="AL46" s="5">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:57">
+      <c r="BR46" s="5">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:91">
       <c r="B47" s="3" t="s">
         <v>22</v>
       </c>
@@ -5125,8 +5800,11 @@
       <c r="AL47" s="5">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:57">
+      <c r="BR47" s="5">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:91">
       <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
@@ -5136,8 +5814,11 @@
       <c r="AL48" s="5">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="49" spans="1:73">
+      <c r="BR48" s="5">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:76">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -5147,8 +5828,11 @@
       <c r="AL49" s="5">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:73">
+      <c r="BR49" s="5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:76">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -5161,8 +5845,11 @@
       <c r="AL51" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="52" spans="1:73">
+      <c r="BR51" s="5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:76">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -5181,11 +5868,17 @@
       <c r="AR52" s="7">
         <v>400</v>
       </c>
+      <c r="BR52" s="5">
+        <v>400</v>
+      </c>
       <c r="BU52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:73">
+      <c r="BX52" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:76">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -5201,11 +5894,17 @@
       <c r="AR53" s="7">
         <v>0</v>
       </c>
+      <c r="BR53" s="5">
+        <v>0</v>
+      </c>
       <c r="BU53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:73">
+      <c r="BX53" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:76">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -5215,8 +5914,12 @@
       <c r="AL54" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="55" spans="1:73">
+      <c r="BR54" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="BX54" s="7"/>
+    </row>
+    <row r="55" spans="1:76">
       <c r="D55" s="11">
         <v>25</v>
       </c>
@@ -5229,11 +5932,17 @@
       <c r="AR55" s="7">
         <v>25</v>
       </c>
+      <c r="BR55" s="5">
+        <v>25</v>
+      </c>
       <c r="BU55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:73">
+      <c r="BX55" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:76">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -5249,11 +5958,17 @@
       <c r="AR56" s="7">
         <v>200</v>
       </c>
+      <c r="BR56" s="5">
+        <v>200</v>
+      </c>
       <c r="BU56">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:73">
+      <c r="BX56" s="7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:76">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -5267,7 +5982,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:73">
+    <row r="59" spans="1:76">
       <c r="L59" t="s">
         <v>350</v>
       </c>
@@ -5284,10 +5999,10 @@
   <dimension ref="A1:ES66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="EG9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="EO7" sqref="EO7"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -11557,7 +12272,7 @@
   <dimension ref="A1:CE69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="K27" sqref="K27"/>

</xml_diff>

<commit_message>
Finalize network parameters; create population analysis
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="435">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1710,6 +1710,38 @@
   </si>
   <si>
     <t>baseline_r43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r43</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_r47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_r47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_r47</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2114,13 +2146,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CM59"/>
+  <dimension ref="A1:CV59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CA9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CJ9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CM21" sqref="CM21"/>
+      <selection pane="bottomRight" activeCell="CT25" sqref="CT25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2149,9 +2181,11 @@
     <col min="87" max="88" width="9" style="7"/>
     <col min="90" max="90" width="9" style="5"/>
     <col min="91" max="91" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="99" max="100" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:91">
+    <row r="1" spans="1:100">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2396,8 +2430,32 @@
       <c r="CM1" s="7" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="2" spans="1:91">
+      <c r="CN1" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="CO1" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="CQ1" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="CR1" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="CS1" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="CT1" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="CU1" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="CV1" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="2" spans="1:100">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2408,7 +2466,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:91">
+    <row r="3" spans="1:100">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2676,8 +2734,38 @@
       <c r="CL3" s="5">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:91">
+      <c r="CM3">
+        <v>1.91</v>
+      </c>
+      <c r="CN3">
+        <v>2.85</v>
+      </c>
+      <c r="CO3">
+        <v>2.04</v>
+      </c>
+      <c r="CP3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="CQ3">
+        <v>1.92</v>
+      </c>
+      <c r="CR3">
+        <v>1.9</v>
+      </c>
+      <c r="CS3">
+        <v>1.9</v>
+      </c>
+      <c r="CT3" s="5">
+        <v>1.9</v>
+      </c>
+      <c r="CU3" s="9">
+        <v>2.86</v>
+      </c>
+      <c r="CV3" s="9">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:100">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2939,8 +3027,38 @@
       <c r="CL4" s="5">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="5" spans="1:91">
+      <c r="CM4">
+        <v>1.81</v>
+      </c>
+      <c r="CN4">
+        <v>1.82</v>
+      </c>
+      <c r="CO4">
+        <v>1.49</v>
+      </c>
+      <c r="CP4" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="CQ4">
+        <v>1.81</v>
+      </c>
+      <c r="CR4">
+        <v>1.8</v>
+      </c>
+      <c r="CS4">
+        <v>1.81</v>
+      </c>
+      <c r="CT4" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="CU4" s="9">
+        <v>1.81</v>
+      </c>
+      <c r="CV4" s="9">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:100">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3205,8 +3323,38 @@
       <c r="CL5" s="5">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:91">
+      <c r="CM5">
+        <v>1.29</v>
+      </c>
+      <c r="CN5">
+        <v>2.15</v>
+      </c>
+      <c r="CO5">
+        <v>2.68</v>
+      </c>
+      <c r="CP5" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="CQ5">
+        <v>1.29</v>
+      </c>
+      <c r="CR5">
+        <v>1.3</v>
+      </c>
+      <c r="CS5">
+        <v>1.3</v>
+      </c>
+      <c r="CT5" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="CU5" s="9">
+        <v>2.17</v>
+      </c>
+      <c r="CV5" s="9">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:100">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3465,8 +3613,38 @@
       <c r="CL6" s="5">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="7" spans="1:91">
+      <c r="CM6">
+        <v>1.37</v>
+      </c>
+      <c r="CN6">
+        <v>1.46</v>
+      </c>
+      <c r="CO6">
+        <v>1.65</v>
+      </c>
+      <c r="CP6" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="CQ6">
+        <v>1.37</v>
+      </c>
+      <c r="CR6">
+        <v>1.38</v>
+      </c>
+      <c r="CS6">
+        <v>1.37</v>
+      </c>
+      <c r="CT6" s="5">
+        <v>1.37</v>
+      </c>
+      <c r="CU6" s="9">
+        <v>1.47</v>
+      </c>
+      <c r="CV6" s="9">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:100">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3731,8 +3909,38 @@
       <c r="CL7" s="5">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:91">
+      <c r="CM7">
+        <v>7.53</v>
+      </c>
+      <c r="CN7">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="CO7">
+        <v>5.04</v>
+      </c>
+      <c r="CP7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="CQ7">
+        <v>7.57</v>
+      </c>
+      <c r="CR7">
+        <v>7.48</v>
+      </c>
+      <c r="CS7">
+        <v>7.49</v>
+      </c>
+      <c r="CT7" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="CU7" s="9">
+        <v>17.7</v>
+      </c>
+      <c r="CV7" s="9">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:100">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -3991,8 +4199,38 @@
       <c r="CL8" s="5">
         <v>6.02</v>
       </c>
-    </row>
-    <row r="9" spans="1:91">
+      <c r="CM8">
+        <v>6.83</v>
+      </c>
+      <c r="CN8">
+        <v>11.3</v>
+      </c>
+      <c r="CO8">
+        <v>5.12</v>
+      </c>
+      <c r="CP8" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="CQ8">
+        <v>6.84</v>
+      </c>
+      <c r="CR8">
+        <v>6.77</v>
+      </c>
+      <c r="CS8">
+        <v>6.8</v>
+      </c>
+      <c r="CT8" s="5">
+        <v>6.78</v>
+      </c>
+      <c r="CU8" s="9">
+        <v>11.4</v>
+      </c>
+      <c r="CV8" s="9">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:100">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4257,8 +4495,38 @@
       <c r="CL9" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:91">
+      <c r="CM9">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="CN9">
+        <v>6.6</v>
+      </c>
+      <c r="CO9">
+        <v>12.9</v>
+      </c>
+      <c r="CP9" s="12">
+        <v>5</v>
+      </c>
+      <c r="CQ9">
+        <v>5</v>
+      </c>
+      <c r="CR9">
+        <v>4.99</v>
+      </c>
+      <c r="CS9">
+        <v>5</v>
+      </c>
+      <c r="CT9" s="5">
+        <v>5.01</v>
+      </c>
+      <c r="CU9" s="9">
+        <v>6.5</v>
+      </c>
+      <c r="CV9" s="9">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:100">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -4517,8 +4785,38 @@
       <c r="CL10" s="5">
         <v>5.93</v>
       </c>
-    </row>
-    <row r="11" spans="1:91">
+      <c r="CM10">
+        <v>5.94</v>
+      </c>
+      <c r="CN10">
+        <v>6.34</v>
+      </c>
+      <c r="CO10">
+        <v>7.26</v>
+      </c>
+      <c r="CP10" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="CQ10">
+        <v>5.91</v>
+      </c>
+      <c r="CR10">
+        <v>5.92</v>
+      </c>
+      <c r="CS10">
+        <v>5.92</v>
+      </c>
+      <c r="CT10" s="5">
+        <v>5.93</v>
+      </c>
+      <c r="CU10" s="9">
+        <v>6.35</v>
+      </c>
+      <c r="CV10" s="9">
+        <v>7.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:100">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -4627,8 +4925,17 @@
       <c r="CJ11" s="7">
         <v>39.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:91">
+      <c r="CN11">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="CU11" s="9">
+        <v>35</v>
+      </c>
+      <c r="CV11" s="9">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:100">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -4734,8 +5041,17 @@
       <c r="CJ12" s="7">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="13" spans="1:91">
+      <c r="CN12">
+        <v>0.6</v>
+      </c>
+      <c r="CU12" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="CV12" s="9">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:100">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -4778,8 +5094,14 @@
       <c r="CB13">
         <v>38.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:91">
+      <c r="CU13" s="9">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="CV13" s="9">
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:100">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -4822,8 +5144,14 @@
       <c r="CB14">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="17" spans="1:91">
+      <c r="CU14" s="9">
+        <v>0.52</v>
+      </c>
+      <c r="CV14" s="9">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:98">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -4902,14 +5230,22 @@
       <c r="CF17">
         <v>8.1300000000000008</v>
       </c>
-      <c r="CI17">
-        <v>8.1300000000000008</v>
-      </c>
+      <c r="CI17"/>
       <c r="CL17" s="5">
         <v>8.1300000000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:91">
+      <c r="CM17" s="7"/>
+      <c r="CR17">
+        <v>8.1</v>
+      </c>
+      <c r="CS17">
+        <v>8.11</v>
+      </c>
+      <c r="CT17" s="5">
+        <v>8.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:98">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -4964,8 +5300,23 @@
       <c r="CL18" s="5">
         <v>12.91</v>
       </c>
-    </row>
-    <row r="19" spans="1:91">
+      <c r="CM18" s="7">
+        <v>12.76</v>
+      </c>
+      <c r="CQ18">
+        <v>12.78</v>
+      </c>
+      <c r="CR18">
+        <v>12.79</v>
+      </c>
+      <c r="CS18">
+        <v>12.8</v>
+      </c>
+      <c r="CT18" s="5">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:98">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -5074,11 +5425,24 @@
       <c r="CL19" s="5">
         <v>0.81299999999999994</v>
       </c>
-      <c r="CM19">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:91">
+      <c r="CM19" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="CN19" s="7"/>
+      <c r="CQ19">
+        <v>1.68</v>
+      </c>
+      <c r="CR19">
+        <v>1.68</v>
+      </c>
+      <c r="CS19">
+        <v>1.68</v>
+      </c>
+      <c r="CT19" s="5">
+        <v>1.6870000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:98">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -5157,16 +5521,29 @@
       <c r="CL20" s="5">
         <v>2.25</v>
       </c>
-      <c r="CM20">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:91">
+      <c r="CM20" s="7">
+        <v>2.23</v>
+      </c>
+      <c r="CQ20">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="CR20">
+        <v>2.222</v>
+      </c>
+      <c r="CS20">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="CT20" s="5">
+        <v>2.2250000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:98">
       <c r="C21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:91">
+      <c r="CM21" s="7"/>
+    </row>
+    <row r="22" spans="1:98">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -5186,13 +5563,17 @@
         <v>3.6</v>
       </c>
       <c r="AL22" s="5">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="BR22" s="5">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:91">
+        <v>3.2</v>
+      </c>
+      <c r="CM22" s="7"/>
+      <c r="CT22" s="5">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:98">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -5214,8 +5595,12 @@
       <c r="BR23" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:91">
+      <c r="CM23" s="7"/>
+      <c r="CT23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:98">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -5237,8 +5622,12 @@
       <c r="BR24" s="5">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:91">
+      <c r="CM24" s="7"/>
+      <c r="CT24" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:98">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -5260,8 +5649,12 @@
       <c r="BR25" s="5">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:91">
+      <c r="CM25" s="7"/>
+      <c r="CT25" s="5">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:98">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -5296,11 +5689,14 @@
       <c r="CL26" s="5">
         <v>9</v>
       </c>
-      <c r="CM26">
+      <c r="CM26" s="7">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:91">
+      <c r="CT26" s="5">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:98">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -5335,11 +5731,14 @@
       <c r="CL27" s="5">
         <v>2</v>
       </c>
-      <c r="CM27">
+      <c r="CM27" s="7">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="28" spans="1:91">
+      <c r="CT27" s="5">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:98">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -5357,16 +5756,17 @@
       </c>
       <c r="M28" s="7"/>
       <c r="AL28" s="5">
-        <v>1.25</v>
+        <v>1.26</v>
       </c>
       <c r="BR28" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="CM28">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:91">
+        <v>1.26</v>
+      </c>
+      <c r="CM28" s="7"/>
+      <c r="CT28" s="5">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:98">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -5389,11 +5789,12 @@
       <c r="BR29" s="5">
         <v>0.53</v>
       </c>
-      <c r="CM29">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:91">
+      <c r="CM29" s="7"/>
+      <c r="CT29" s="5">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:98">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -5413,8 +5814,12 @@
       <c r="BR30" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:91">
+      <c r="CM30" s="7"/>
+      <c r="CT30" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:98">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -5434,8 +5839,12 @@
       <c r="BR31" s="5">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="32" spans="1:91">
+      <c r="CM31" s="7"/>
+      <c r="CT31" s="5">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:98">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -5458,8 +5867,12 @@
       <c r="BR32" s="5">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="33" spans="1:91">
+      <c r="CM32" s="7"/>
+      <c r="CT32" s="5">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:98">
       <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
@@ -5482,8 +5895,12 @@
       <c r="BR33" s="5">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:91">
+      <c r="CM33" s="7"/>
+      <c r="CT33" s="5">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:98">
       <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
@@ -5518,8 +5935,12 @@
       <c r="BR34" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:91">
+      <c r="CM34" s="7"/>
+      <c r="CT34" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:98">
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
@@ -5549,13 +5970,17 @@
         <v>8</v>
       </c>
       <c r="AL35" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BR35" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:91">
+        <v>7</v>
+      </c>
+      <c r="CM35" s="7"/>
+      <c r="CT35" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:98">
       <c r="B36" s="3" t="s">
         <v>31</v>
       </c>
@@ -5587,8 +6012,12 @@
       <c r="BR36" s="5">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:91">
+      <c r="CM36" s="7"/>
+      <c r="CT36" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:98">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -5617,13 +6046,18 @@
       <c r="BR37" s="5">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:91">
+      <c r="CM37" s="7"/>
+      <c r="CT37" s="5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:98">
       <c r="C38" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:91">
+      <c r="CM38" s="7"/>
+    </row>
+    <row r="39" spans="1:98">
       <c r="A39" s="3" t="s">
         <v>213</v>
       </c>
@@ -5666,11 +6100,14 @@
       <c r="CL39" s="5">
         <v>3.3000000000000003E-5</v>
       </c>
-      <c r="CM39">
+      <c r="CM39" s="7">
         <v>6.6000000000000005E-5</v>
       </c>
-    </row>
-    <row r="40" spans="1:91">
+      <c r="CT39" s="5">
+        <v>6.6000000000000005E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:98">
       <c r="B40" s="3" t="s">
         <v>215</v>
       </c>
@@ -5704,11 +6141,14 @@
       <c r="CL40" s="5">
         <v>7.6000000000000004E-4</v>
       </c>
-      <c r="CM40">
-        <v>3.8000000000000002E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:91">
+      <c r="CM40" s="7">
+        <v>7.6000000000000004E-4</v>
+      </c>
+      <c r="CT40" s="5">
+        <v>7.6000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:98">
       <c r="A42" s="3" t="s">
         <v>82</v>
       </c>
@@ -5724,8 +6164,14 @@
       <c r="BR42" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:91">
+      <c r="CL42" s="5">
+        <v>7</v>
+      </c>
+      <c r="CT42" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:98">
       <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
@@ -5741,8 +6187,14 @@
       <c r="BR43" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:91">
+      <c r="CL43" s="5">
+        <v>30</v>
+      </c>
+      <c r="CT43" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:98">
       <c r="B44" s="3" t="s">
         <v>84</v>
       </c>
@@ -5755,8 +6207,14 @@
       <c r="BR44" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:91">
+      <c r="CL44" s="5">
+        <v>5</v>
+      </c>
+      <c r="CT44" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:98">
       <c r="B45" s="3" t="s">
         <v>85</v>
       </c>
@@ -5772,8 +6230,14 @@
       <c r="BR45" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:91">
+      <c r="CL45" s="5">
+        <v>20</v>
+      </c>
+      <c r="CT45" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:98">
       <c r="A46" s="3" t="s">
         <v>82</v>
       </c>
@@ -5789,8 +6253,14 @@
       <c r="BR46" s="5">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:91">
+      <c r="CL46" s="5">
+        <v>2.9</v>
+      </c>
+      <c r="CT46" s="5">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:98">
       <c r="B47" s="3" t="s">
         <v>22</v>
       </c>
@@ -5803,8 +6273,14 @@
       <c r="BR47" s="5">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:91">
+      <c r="CL47" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="CT47" s="5">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:98">
       <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
@@ -5817,8 +6293,14 @@
       <c r="BR48" s="5">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="49" spans="1:76">
+      <c r="CL48" s="5">
+        <v>3.9</v>
+      </c>
+      <c r="CT48" s="5">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:98">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -5831,8 +6313,14 @@
       <c r="BR49" s="5">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:76">
+      <c r="CL49" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="CT49" s="5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:98">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -5848,8 +6336,14 @@
       <c r="BR51" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="52" spans="1:76">
+      <c r="CL51" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="CT51" s="5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:98">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -5877,8 +6371,14 @@
       <c r="BX52" s="7">
         <v>400</v>
       </c>
-    </row>
-    <row r="53" spans="1:76">
+      <c r="CL52" s="5">
+        <v>400</v>
+      </c>
+      <c r="CT52" s="5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:98">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -5903,8 +6403,14 @@
       <c r="BX53" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:76">
+      <c r="CL53" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:98">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -5918,8 +6424,14 @@
         <v>0.3</v>
       </c>
       <c r="BX54" s="7"/>
-    </row>
-    <row r="55" spans="1:76">
+      <c r="CL54" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="CT54" s="5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:98">
       <c r="D55" s="11">
         <v>25</v>
       </c>
@@ -5941,8 +6453,14 @@
       <c r="BX55" s="7">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:76">
+      <c r="CL55" s="5">
+        <v>25</v>
+      </c>
+      <c r="CT55" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:98">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -5967,8 +6485,14 @@
       <c r="BX56" s="7">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:76">
+      <c r="CL56" s="5">
+        <v>200</v>
+      </c>
+      <c r="CT56" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:98">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -5982,7 +6506,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="59" spans="1:76">
+    <row r="59" spans="1:98">
       <c r="L59" t="s">
         <v>350</v>
       </c>

</xml_diff>

<commit_message>
Add method of assigning assemblies in grids; add grid assembly results
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="440">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1742,6 +1742,26 @@
   </si>
   <si>
     <t>long_r47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_grid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_grid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2146,13 +2166,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CV59"/>
+  <dimension ref="A1:DA59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CJ9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CR3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CT25" sqref="CT25"/>
+      <selection pane="bottomRight" activeCell="DB9" sqref="DB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2183,9 +2203,11 @@
     <col min="91" max="91" width="9.5" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="9.5" style="5" bestFit="1" customWidth="1"/>
     <col min="99" max="100" width="9" style="9"/>
+    <col min="101" max="101" width="9" style="5"/>
+    <col min="102" max="105" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100">
+    <row r="1" spans="1:105">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2454,8 +2476,23 @@
       <c r="CV1" s="9" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="2" spans="1:100">
+      <c r="CW1" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="CX1" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="CY1" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="CZ1" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="DA1" s="9" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="2" spans="1:105">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2466,7 +2503,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:100">
+    <row r="3" spans="1:105">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2764,8 +2801,23 @@
       <c r="CV3" s="9">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:100">
+      <c r="CW3" s="5">
+        <v>1.92</v>
+      </c>
+      <c r="CX3" s="9">
+        <v>2.94</v>
+      </c>
+      <c r="CY3" s="9">
+        <v>2.04</v>
+      </c>
+      <c r="CZ3" s="9">
+        <v>2.67</v>
+      </c>
+      <c r="DA3" s="9">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:105">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3057,8 +3109,23 @@
       <c r="CV4" s="9">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="5" spans="1:100">
+      <c r="CW4" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="CX4" s="9">
+        <v>1.83</v>
+      </c>
+      <c r="CY4" s="9">
+        <v>1.49</v>
+      </c>
+      <c r="CZ4" s="9">
+        <v>1.81</v>
+      </c>
+      <c r="DA4" s="9">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:105">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3353,8 +3420,23 @@
       <c r="CV5" s="9">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:100">
+      <c r="CW5" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="CX5" s="9">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="CY5" s="9">
+        <v>2.81</v>
+      </c>
+      <c r="CZ5" s="9">
+        <v>1.99</v>
+      </c>
+      <c r="DA5" s="9">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:105">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3643,8 +3725,23 @@
       <c r="CV6" s="9">
         <v>1.66</v>
       </c>
-    </row>
-    <row r="7" spans="1:100">
+      <c r="CW6" s="5">
+        <v>1.38</v>
+      </c>
+      <c r="CX6" s="9">
+        <v>1.51</v>
+      </c>
+      <c r="CY6" s="9">
+        <v>1.71</v>
+      </c>
+      <c r="CZ6" s="9">
+        <v>1.52</v>
+      </c>
+      <c r="DA6" s="9">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:105">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3939,8 +4036,23 @@
       <c r="CV7" s="9">
         <v>4.99</v>
       </c>
-    </row>
-    <row r="8" spans="1:100">
+      <c r="CW7" s="5">
+        <v>7.88</v>
+      </c>
+      <c r="CX7" s="9">
+        <v>18.8</v>
+      </c>
+      <c r="CY7" s="9">
+        <v>5.12</v>
+      </c>
+      <c r="CZ7" s="9">
+        <v>15.6</v>
+      </c>
+      <c r="DA7" s="9">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:105">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -4229,8 +4341,23 @@
       <c r="CV8" s="9">
         <v>5.04</v>
       </c>
-    </row>
-    <row r="9" spans="1:100">
+      <c r="CW8" s="5">
+        <v>7.12</v>
+      </c>
+      <c r="CX8" s="9">
+        <v>12</v>
+      </c>
+      <c r="CY8" s="9">
+        <v>5.12</v>
+      </c>
+      <c r="CZ8" s="9">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="DA8" s="9">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:105">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4525,8 +4652,23 @@
       <c r="CV9" s="9">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:100">
+      <c r="CW9" s="5">
+        <v>5.13</v>
+      </c>
+      <c r="CX9" s="9">
+        <v>7.08</v>
+      </c>
+      <c r="CY9" s="9">
+        <v>13.9</v>
+      </c>
+      <c r="CZ9" s="9">
+        <v>6.94</v>
+      </c>
+      <c r="DA9" s="9">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:105">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -4815,8 +4957,23 @@
       <c r="CV10" s="9">
         <v>7.21</v>
       </c>
-    </row>
-    <row r="11" spans="1:100">
+      <c r="CW10" s="5">
+        <v>6.11</v>
+      </c>
+      <c r="CX10" s="9">
+        <v>6.47</v>
+      </c>
+      <c r="CY10" s="9">
+        <v>7.43</v>
+      </c>
+      <c r="CZ10" s="9">
+        <v>5.99</v>
+      </c>
+      <c r="DA10" s="9">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:105">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -4934,8 +5091,20 @@
       <c r="CV11" s="9">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:100">
+      <c r="CX11" s="9">
+        <v>38.6</v>
+      </c>
+      <c r="CY11" s="9">
+        <v>17.8</v>
+      </c>
+      <c r="CZ11" s="9">
+        <v>37.4</v>
+      </c>
+      <c r="DA11" s="9">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:105">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -5050,8 +5219,20 @@
       <c r="CV12" s="9">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="13" spans="1:100">
+      <c r="CX12" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="CY12" s="9">
+        <v>0.86</v>
+      </c>
+      <c r="CZ12" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="DA12" s="9">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:105">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -5100,8 +5281,14 @@
       <c r="CV13" s="9">
         <v>37.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:100">
+      <c r="CY13" s="9">
+        <v>38.1</v>
+      </c>
+      <c r="CZ13" s="9">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:105">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -5149,6 +5336,12 @@
       </c>
       <c r="CV14" s="9">
         <v>0.45</v>
+      </c>
+      <c r="CY14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="CZ14" s="9">
+        <v>0.64</v>
       </c>
     </row>
     <row r="17" spans="1:98">

</xml_diff>

<commit_message>
Simplify STP synapses modfiles; fix error in PSG random seed; create input to divided intrinsics assemblies
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="recover" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="447">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1745,15 +1745,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>baseline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>short</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>long</t>
+    <t>short_grid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New connectivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>with assemblies</t>
+  </si>
+  <si>
+    <t>baseline_rand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_rand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_rand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_div</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_div</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_grid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_grid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2166,13 +2193,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DA59"/>
+  <dimension ref="A1:DL59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CR3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CS3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DB9" sqref="DB9"/>
+      <selection pane="bottomRight" activeCell="DD20" sqref="DD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2203,11 +2230,13 @@
     <col min="91" max="91" width="9.5" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="9.5" style="5" bestFit="1" customWidth="1"/>
     <col min="99" max="100" width="9" style="9"/>
-    <col min="101" max="101" width="9" style="5"/>
-    <col min="102" max="105" width="9" style="9"/>
+    <col min="102" max="102" width="9" style="5"/>
+    <col min="103" max="106" width="9" style="9"/>
+    <col min="107" max="108" width="9" style="7"/>
+    <col min="110" max="116" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105">
+    <row r="1" spans="1:116">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2476,23 +2505,44 @@
       <c r="CV1" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="CW1" s="5" t="s">
+      <c r="CX1" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="CY1" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="CZ1" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="DA1" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="DB1" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="DC1" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="DD1" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="DH1" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="DI1" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="DJ1" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="DK1" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="CX1" s="9" t="s">
-        <v>436</v>
-      </c>
-      <c r="CY1" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="CZ1" s="9" t="s">
-        <v>438</v>
-      </c>
-      <c r="DA1" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="2" spans="1:105">
+      <c r="DL1" s="7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:116">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2503,7 +2553,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:105">
+    <row r="3" spans="1:116">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2801,23 +2851,32 @@
       <c r="CV3" s="9">
         <v>2.0299999999999998</v>
       </c>
-      <c r="CW3" s="5">
-        <v>1.92</v>
-      </c>
-      <c r="CX3" s="9">
-        <v>2.94</v>
+      <c r="CW3" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="CX3" s="5">
+        <v>1.9</v>
       </c>
       <c r="CY3" s="9">
-        <v>2.04</v>
+        <v>2.88</v>
       </c>
       <c r="CZ3" s="9">
-        <v>2.67</v>
+        <v>1.97</v>
       </c>
       <c r="DA3" s="9">
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:105">
+        <v>2.91</v>
+      </c>
+      <c r="DB3" s="9">
+        <v>1.97</v>
+      </c>
+      <c r="DC3" s="7">
+        <v>2.62</v>
+      </c>
+      <c r="DD3" s="7">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:116">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3109,23 +3168,32 @@
       <c r="CV4" s="9">
         <v>1.48</v>
       </c>
-      <c r="CW4" s="5">
+      <c r="CW4" s="12">
         <v>1.8</v>
       </c>
-      <c r="CX4" s="9">
-        <v>1.83</v>
+      <c r="CX4" s="5">
+        <v>1.82</v>
       </c>
       <c r="CY4" s="9">
-        <v>1.49</v>
+        <v>1.86</v>
       </c>
       <c r="CZ4" s="9">
-        <v>1.81</v>
+        <v>1.57</v>
       </c>
       <c r="DA4" s="9">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:105">
+        <v>1.88</v>
+      </c>
+      <c r="DB4" s="9">
+        <v>1.54</v>
+      </c>
+      <c r="DC4" s="7">
+        <v>1.85</v>
+      </c>
+      <c r="DD4" s="7">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:116">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3420,23 +3488,32 @@
       <c r="CV5" s="9">
         <v>2.7</v>
       </c>
-      <c r="CW5" s="5">
+      <c r="CW5" s="12">
         <v>1.3</v>
       </c>
-      <c r="CX5" s="9">
-        <v>2.2799999999999998</v>
+      <c r="CX5" s="5">
+        <v>1.3</v>
       </c>
       <c r="CY5" s="9">
-        <v>2.81</v>
+        <v>2.31</v>
       </c>
       <c r="CZ5" s="9">
-        <v>1.99</v>
+        <v>2.82</v>
       </c>
       <c r="DA5" s="9">
-        <v>2.57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:105">
+        <v>2.33</v>
+      </c>
+      <c r="DB5" s="9">
+        <v>2.83</v>
+      </c>
+      <c r="DC5" s="7">
+        <v>2.02</v>
+      </c>
+      <c r="DD5" s="7">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:116">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3725,23 +3802,32 @@
       <c r="CV6" s="9">
         <v>1.66</v>
       </c>
-      <c r="CW6" s="5">
-        <v>1.38</v>
-      </c>
-      <c r="CX6" s="9">
+      <c r="CW6" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="CX6" s="5">
+        <v>1.37</v>
+      </c>
+      <c r="CY6" s="9">
+        <v>1.52</v>
+      </c>
+      <c r="CZ6" s="9">
+        <v>1.73</v>
+      </c>
+      <c r="DA6" s="9">
         <v>1.51</v>
       </c>
-      <c r="CY6" s="9">
-        <v>1.71</v>
-      </c>
-      <c r="CZ6" s="9">
-        <v>1.52</v>
-      </c>
-      <c r="DA6" s="9">
+      <c r="DB6" s="9">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="7" spans="1:105">
+      <c r="DC6" s="7">
+        <v>1.55</v>
+      </c>
+      <c r="DD6" s="7">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:116">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4036,23 +4122,32 @@
       <c r="CV7" s="9">
         <v>4.99</v>
       </c>
-      <c r="CW7" s="5">
-        <v>7.88</v>
-      </c>
-      <c r="CX7" s="9">
-        <v>18.8</v>
+      <c r="CW7" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="CX7" s="5">
+        <v>7.52</v>
       </c>
       <c r="CY7" s="9">
-        <v>5.12</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="CZ7" s="9">
-        <v>15.6</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="DA7" s="9">
-        <v>6.57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:105">
+        <v>18.3</v>
+      </c>
+      <c r="DB7" s="9">
+        <v>4.43</v>
+      </c>
+      <c r="DC7" s="7">
+        <v>15.1</v>
+      </c>
+      <c r="DD7" s="7">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:116">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -4341,23 +4436,32 @@
       <c r="CV8" s="9">
         <v>5.04</v>
       </c>
-      <c r="CW8" s="5">
-        <v>7.12</v>
-      </c>
-      <c r="CX8" s="9">
-        <v>12</v>
+      <c r="CW8" s="12">
+        <v>6.4</v>
+      </c>
+      <c r="CX8" s="5">
+        <v>6.38</v>
       </c>
       <c r="CY8" s="9">
+        <v>11.1</v>
+      </c>
+      <c r="CZ8" s="9">
+        <v>4.17</v>
+      </c>
+      <c r="DA8" s="9">
+        <v>11.2</v>
+      </c>
+      <c r="DB8" s="9">
+        <v>4.09</v>
+      </c>
+      <c r="DC8" s="7">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="DD8" s="7">
         <v>5.12</v>
       </c>
-      <c r="CZ8" s="9">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="DA8" s="9">
-        <v>5.89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:105">
+    </row>
+    <row r="9" spans="1:116">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4652,23 +4756,32 @@
       <c r="CV9" s="9">
         <v>12.9</v>
       </c>
-      <c r="CW9" s="5">
-        <v>5.13</v>
-      </c>
-      <c r="CX9" s="9">
-        <v>7.08</v>
+      <c r="CW9" s="12">
+        <v>5</v>
+      </c>
+      <c r="CX9" s="5">
+        <v>5</v>
       </c>
       <c r="CY9" s="9">
-        <v>13.9</v>
+        <v>7.01</v>
       </c>
       <c r="CZ9" s="9">
-        <v>6.94</v>
+        <v>14.2</v>
       </c>
       <c r="DA9" s="9">
-        <v>11.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:105">
+        <v>7.1</v>
+      </c>
+      <c r="DB9" s="9">
+        <v>14.5</v>
+      </c>
+      <c r="DC9" s="7">
+        <v>6.91</v>
+      </c>
+      <c r="DD9" s="7">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:116">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -4957,23 +5070,32 @@
       <c r="CV10" s="9">
         <v>7.21</v>
       </c>
-      <c r="CW10" s="5">
-        <v>6.11</v>
-      </c>
-      <c r="CX10" s="9">
-        <v>6.47</v>
+      <c r="CW10" s="12">
+        <v>6</v>
+      </c>
+      <c r="CX10" s="5">
+        <v>5.9</v>
       </c>
       <c r="CY10" s="9">
-        <v>7.43</v>
+        <v>6.36</v>
       </c>
       <c r="CZ10" s="9">
-        <v>5.99</v>
+        <v>7.11</v>
       </c>
       <c r="DA10" s="9">
-        <v>6.31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:105">
+        <v>6.39</v>
+      </c>
+      <c r="DB10" s="9">
+        <v>7.11</v>
+      </c>
+      <c r="DC10" s="7">
+        <v>6.07</v>
+      </c>
+      <c r="DD10" s="7">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:116">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5091,20 +5213,26 @@
       <c r="CV11" s="9">
         <v>18.5</v>
       </c>
-      <c r="CX11" s="9">
-        <v>38.6</v>
-      </c>
       <c r="CY11" s="9">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="CZ11" s="9">
         <v>17.8</v>
       </c>
-      <c r="CZ11" s="9">
-        <v>37.4</v>
-      </c>
       <c r="DA11" s="9">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:105">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="DB11" s="9">
+        <v>17.7</v>
+      </c>
+      <c r="DC11" s="7">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="DD11" s="7">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:116">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -5219,20 +5347,26 @@
       <c r="CV12" s="9">
         <v>0.48</v>
       </c>
-      <c r="CX12" s="9">
-        <v>0.53</v>
-      </c>
       <c r="CY12" s="9">
-        <v>0.86</v>
+        <v>0.36</v>
       </c>
       <c r="CZ12" s="9">
+        <v>0.97</v>
+      </c>
+      <c r="DA12" s="9">
         <v>0.68</v>
       </c>
-      <c r="DA12" s="9">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:105">
+      <c r="DB12" s="9">
+        <v>1</v>
+      </c>
+      <c r="DC12" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="DD12" s="7">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:116">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -5281,14 +5415,17 @@
       <c r="CV13" s="9">
         <v>37.1</v>
       </c>
-      <c r="CY13" s="9">
-        <v>38.1</v>
-      </c>
       <c r="CZ13" s="9">
-        <v>45.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:105">
+        <v>37.5</v>
+      </c>
+      <c r="DB13" s="9">
+        <v>37.9</v>
+      </c>
+      <c r="DC13" s="7">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:116">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -5337,14 +5474,27 @@
       <c r="CV14" s="9">
         <v>0.45</v>
       </c>
-      <c r="CY14" s="9">
+      <c r="CZ14" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="DB14" s="9">
+        <v>0.48</v>
+      </c>
+      <c r="DC14" s="7">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:116">
+      <c r="DC15" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:116">
+      <c r="DC16" s="7">
         <v>0.5</v>
       </c>
-      <c r="CZ14" s="9">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:98">
+    </row>
+    <row r="17" spans="1:102">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -5437,8 +5587,11 @@
       <c r="CT17" s="5">
         <v>8.11</v>
       </c>
-    </row>
-    <row r="18" spans="1:98">
+      <c r="CX17" s="5">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:102">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -5508,8 +5661,11 @@
       <c r="CT18" s="5">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:98">
+      <c r="CX18" s="5">
+        <v>12.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:102">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -5634,8 +5790,11 @@
       <c r="CT19" s="5">
         <v>1.6870000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:98">
+      <c r="CX19" s="5">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:102">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -5729,14 +5888,17 @@
       <c r="CT20" s="5">
         <v>2.2250000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:98">
+      <c r="CX20" s="5">
+        <v>2.2240000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:102">
       <c r="C21" t="s">
         <v>32</v>
       </c>
       <c r="CM21" s="7"/>
     </row>
-    <row r="22" spans="1:98">
+    <row r="22" spans="1:102">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -5766,7 +5928,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="23" spans="1:98">
+    <row r="23" spans="1:102">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -5793,7 +5955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:98">
+    <row r="24" spans="1:102">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -5820,7 +5982,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:98">
+    <row r="25" spans="1:102">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -5847,7 +6009,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:98">
+    <row r="26" spans="1:102">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -5889,7 +6051,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="27" spans="1:98">
+    <row r="27" spans="1:102">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -5931,7 +6093,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="28" spans="1:98">
+    <row r="28" spans="1:102">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -5959,7 +6121,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="29" spans="1:98">
+    <row r="29" spans="1:102">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -5987,7 +6149,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="30" spans="1:98">
+    <row r="30" spans="1:102">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -6012,7 +6174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:98">
+    <row r="31" spans="1:102">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -6037,7 +6199,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="32" spans="1:98">
+    <row r="32" spans="1:102">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -6493,7 +6655,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="49" spans="1:98">
+    <row r="49" spans="1:101">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -6513,7 +6675,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="51" spans="1:98">
+    <row r="51" spans="1:101">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -6536,7 +6698,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:98">
+    <row r="52" spans="1:101">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -6571,7 +6733,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="53" spans="1:98">
+    <row r="53" spans="1:101">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -6603,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:98">
+    <row r="54" spans="1:101">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -6624,7 +6786,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="55" spans="1:98">
+    <row r="55" spans="1:101">
       <c r="D55" s="11">
         <v>25</v>
       </c>
@@ -6653,7 +6815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:98">
+    <row r="56" spans="1:101">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -6685,7 +6847,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="1:98">
+    <row r="58" spans="1:101">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -6698,10 +6860,16 @@
       <c r="AR58" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="59" spans="1:98">
+      <c r="CW58" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="59" spans="1:101">
       <c r="L59" t="s">
         <v>350</v>
+      </c>
+      <c r="CW59" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pipeline; Correct background input weights
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="448">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1777,6 +1777,22 @@
   </si>
   <si>
     <t>long_grid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_rand_single_assembly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_div_single_assembly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_validate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200 Hz</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1801,7 +1817,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1832,6 +1848,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1847,7 +1869,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1885,6 +1907,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2184,10 +2209,10 @@
   <dimension ref="A1:DL59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CR3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CV3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CZ13" sqref="CZ13"/>
+      <selection pane="bottomRight" activeCell="DE12" sqref="DE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2219,12 +2244,14 @@
     <col min="98" max="98" width="9.5" style="5" bestFit="1" customWidth="1"/>
     <col min="99" max="100" width="9" style="9"/>
     <col min="102" max="102" width="9" style="5"/>
-    <col min="103" max="106" width="9" style="9"/>
-    <col min="107" max="108" width="9" style="7"/>
+    <col min="103" max="104" width="9" style="9"/>
+    <col min="105" max="105" width="9" style="13"/>
+    <col min="106" max="107" width="9" style="9"/>
+    <col min="108" max="108" width="9" style="13"/>
     <col min="110" max="116" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:108">
+    <row r="1" spans="1:113">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2502,20 +2529,29 @@
       <c r="CZ1" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="DA1" s="9" t="s">
+      <c r="DA1" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="DB1" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="DB1" s="9" t="s">
+      <c r="DC1" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="DC1" s="7" t="s">
+      <c r="DD1" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="DF1" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="DD1" s="7" t="s">
+      <c r="DG1" s="7" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="2" spans="1:108">
+      <c r="DI1" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:113">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2526,7 +2562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:108">
+    <row r="3" spans="1:113">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2836,20 +2872,29 @@
       <c r="CZ3" s="9">
         <v>1.97</v>
       </c>
-      <c r="DA3" s="9">
+      <c r="DA3" s="13">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="DB3" s="9">
         <v>2.91</v>
       </c>
-      <c r="DB3" s="9">
+      <c r="DC3" s="9">
         <v>1.97</v>
       </c>
-      <c r="DC3" s="7">
+      <c r="DD3" s="13">
+        <v>1.93</v>
+      </c>
+      <c r="DF3" s="7">
         <v>2.62</v>
       </c>
-      <c r="DD3" s="7">
+      <c r="DG3" s="7">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:108">
+      <c r="DI3" s="7">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:113">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3153,20 +3198,29 @@
       <c r="CZ4" s="9">
         <v>1.57</v>
       </c>
-      <c r="DA4" s="9">
+      <c r="DA4" s="13">
+        <v>3.89</v>
+      </c>
+      <c r="DB4" s="9">
         <v>1.88</v>
       </c>
-      <c r="DB4" s="9">
+      <c r="DC4" s="9">
         <v>1.54</v>
       </c>
-      <c r="DC4" s="7">
+      <c r="DD4" s="13">
+        <v>3.73</v>
+      </c>
+      <c r="DF4" s="7">
         <v>1.85</v>
       </c>
-      <c r="DD4" s="7">
+      <c r="DG4" s="7">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:108">
+      <c r="DI4" s="7">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:113">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3473,20 +3527,29 @@
       <c r="CZ5" s="9">
         <v>2.82</v>
       </c>
-      <c r="DA5" s="9">
+      <c r="DA5" s="13">
+        <v>2.87</v>
+      </c>
+      <c r="DB5" s="9">
         <v>2.33</v>
       </c>
-      <c r="DB5" s="9">
+      <c r="DC5" s="9">
         <v>2.83</v>
       </c>
-      <c r="DC5" s="7">
+      <c r="DD5" s="13">
+        <v>2.9</v>
+      </c>
+      <c r="DF5" s="7">
         <v>2.02</v>
       </c>
-      <c r="DD5" s="7">
+      <c r="DG5" s="7">
         <v>2.61</v>
       </c>
-    </row>
-    <row r="6" spans="1:108">
+      <c r="DI5" s="7">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:113">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3787,20 +3850,29 @@
       <c r="CZ6" s="9">
         <v>1.73</v>
       </c>
-      <c r="DA6" s="9">
+      <c r="DA6" s="13">
+        <v>5.58</v>
+      </c>
+      <c r="DB6" s="9">
         <v>1.51</v>
       </c>
-      <c r="DB6" s="9">
+      <c r="DC6" s="9">
         <v>1.72</v>
       </c>
-      <c r="DC6" s="7">
+      <c r="DD6" s="13">
+        <v>5.61</v>
+      </c>
+      <c r="DF6" s="7">
         <v>1.55</v>
       </c>
-      <c r="DD6" s="7">
+      <c r="DG6" s="7">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="7" spans="1:108">
+      <c r="DI6" s="7">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:113">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4107,20 +4179,29 @@
       <c r="CZ7" s="9">
         <v>4.5199999999999996</v>
       </c>
-      <c r="DA7" s="9">
+      <c r="DA7" s="13">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="DB7" s="9">
         <v>18.3</v>
       </c>
-      <c r="DB7" s="9">
+      <c r="DC7" s="9">
         <v>4.43</v>
       </c>
-      <c r="DC7" s="7">
+      <c r="DD7" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="DF7" s="7">
         <v>15.1</v>
       </c>
-      <c r="DD7" s="7">
+      <c r="DG7" s="7">
         <v>5.91</v>
       </c>
-    </row>
-    <row r="8" spans="1:108">
+      <c r="DI7" s="7">
+        <v>30.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:113">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -4421,20 +4502,29 @@
       <c r="CZ8" s="9">
         <v>4.17</v>
       </c>
-      <c r="DA8" s="9">
+      <c r="DA8" s="13">
+        <v>4.45</v>
+      </c>
+      <c r="DB8" s="9">
         <v>11.2</v>
       </c>
-      <c r="DB8" s="9">
+      <c r="DC8" s="9">
         <v>4.09</v>
       </c>
-      <c r="DC8" s="7">
+      <c r="DD8" s="13">
+        <v>3.87</v>
+      </c>
+      <c r="DF8" s="7">
         <v>8.5399999999999991</v>
       </c>
-      <c r="DD8" s="7">
+      <c r="DG8" s="7">
         <v>5.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:108">
+      <c r="DI8" s="7">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:113">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4741,20 +4831,29 @@
       <c r="CZ9" s="9">
         <v>14.2</v>
       </c>
-      <c r="DA9" s="9">
+      <c r="DA9" s="13">
+        <v>15.1</v>
+      </c>
+      <c r="DB9" s="9">
         <v>7.1</v>
       </c>
-      <c r="DB9" s="9">
+      <c r="DC9" s="9">
         <v>14.5</v>
       </c>
-      <c r="DC9" s="7">
+      <c r="DD9" s="13">
+        <v>15</v>
+      </c>
+      <c r="DF9" s="7">
         <v>6.91</v>
       </c>
-      <c r="DD9" s="7">
+      <c r="DG9" s="7">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:108">
+      <c r="DI9" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:113">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -5055,20 +5154,29 @@
       <c r="CZ10" s="9">
         <v>7.11</v>
       </c>
-      <c r="DA10" s="9">
+      <c r="DA10" s="13">
+        <v>8.4</v>
+      </c>
+      <c r="DB10" s="9">
         <v>6.39</v>
       </c>
-      <c r="DB10" s="9">
+      <c r="DC10" s="9">
         <v>7.11</v>
       </c>
-      <c r="DC10" s="7">
+      <c r="DD10" s="13">
+        <v>7.91</v>
+      </c>
+      <c r="DF10" s="7">
         <v>6.07</v>
       </c>
-      <c r="DD10" s="7">
+      <c r="DG10" s="7">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:108">
+      <c r="DI10" s="7">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:113">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5192,20 +5300,26 @@
       <c r="CZ11" s="9">
         <v>17.8</v>
       </c>
-      <c r="DA11" s="9">
+      <c r="DA11" s="13">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="DB11" s="9">
         <v>39.200000000000003</v>
       </c>
-      <c r="DB11" s="9">
+      <c r="DC11" s="9">
         <v>17.7</v>
       </c>
-      <c r="DC11" s="7">
+      <c r="DD11" s="13">
+        <v>17.5</v>
+      </c>
+      <c r="DF11" s="7">
         <v>36.299999999999997</v>
       </c>
-      <c r="DD11" s="7">
+      <c r="DG11" s="7">
         <v>41.4</v>
       </c>
     </row>
-    <row r="12" spans="1:108">
+    <row r="12" spans="1:113">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -5326,20 +5440,26 @@
       <c r="CZ12" s="9">
         <v>0.97</v>
       </c>
-      <c r="DA12" s="9">
+      <c r="DA12" s="13">
+        <v>1.01</v>
+      </c>
+      <c r="DB12" s="9">
         <v>0.68</v>
       </c>
-      <c r="DB12" s="9">
+      <c r="DC12" s="9">
         <v>1</v>
       </c>
-      <c r="DC12" s="7">
+      <c r="DD12" s="13">
+        <v>1.05</v>
+      </c>
+      <c r="DF12" s="7">
         <v>0.59</v>
       </c>
-      <c r="DD12" s="7">
+      <c r="DG12" s="7">
         <v>0.59</v>
       </c>
     </row>
-    <row r="13" spans="1:108">
+    <row r="13" spans="1:113">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -5391,14 +5511,20 @@
       <c r="CZ13" s="9">
         <v>37.5</v>
       </c>
-      <c r="DB13" s="9">
+      <c r="DA13" s="13">
+        <v>36.5</v>
+      </c>
+      <c r="DC13" s="9">
         <v>37.9</v>
       </c>
-      <c r="DC13" s="7">
+      <c r="DD13" s="13">
+        <v>36.9</v>
+      </c>
+      <c r="DF13" s="7">
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:108">
+    <row r="14" spans="1:113">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -5450,24 +5576,30 @@
       <c r="CZ14" s="9">
         <v>0.39</v>
       </c>
-      <c r="DB14" s="9">
+      <c r="DA14" s="13">
+        <v>0.44</v>
+      </c>
+      <c r="DC14" s="9">
         <v>0.48</v>
       </c>
-      <c r="DC14" s="7">
+      <c r="DD14" s="13">
+        <v>0.36</v>
+      </c>
+      <c r="DF14" s="7">
         <v>0.59</v>
       </c>
     </row>
-    <row r="15" spans="1:108">
-      <c r="DC15" s="7">
+    <row r="15" spans="1:113">
+      <c r="DF15" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:108">
-      <c r="DC16" s="7">
+    <row r="16" spans="1:113">
+      <c r="DF16" s="7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:102">
+    <row r="17" spans="1:113">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -5564,7 +5696,7 @@
         <v>8.01</v>
       </c>
     </row>
-    <row r="18" spans="1:102">
+    <row r="18" spans="1:113">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -5638,7 +5770,7 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="19" spans="1:102">
+    <row r="19" spans="1:113">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -5766,8 +5898,11 @@
       <c r="CX19" s="5">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="20" spans="1:102">
+      <c r="DI19" s="7">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:113">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -5865,13 +6000,16 @@
         <v>2.2240000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:102">
+    <row r="21" spans="1:113">
       <c r="C21" t="s">
         <v>32</v>
       </c>
       <c r="CM21" s="7"/>
-    </row>
-    <row r="22" spans="1:102">
+      <c r="DI21" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:113">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -5901,7 +6039,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="23" spans="1:102">
+    <row r="23" spans="1:113">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -5928,7 +6066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:102">
+    <row r="24" spans="1:113">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -5955,7 +6093,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:102">
+    <row r="25" spans="1:113">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -5982,7 +6120,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:102">
+    <row r="26" spans="1:113">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -6023,8 +6161,11 @@
       <c r="CT26" s="5">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:102">
+      <c r="DI26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:113">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -6065,8 +6206,11 @@
       <c r="CT27" s="5">
         <v>1.88</v>
       </c>
-    </row>
-    <row r="28" spans="1:102">
+      <c r="DI27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:113">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -6094,7 +6238,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="29" spans="1:102">
+    <row r="29" spans="1:113">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -6122,7 +6266,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="30" spans="1:102">
+    <row r="30" spans="1:113">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -6147,7 +6291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:102">
+    <row r="31" spans="1:113">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -6172,7 +6316,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="32" spans="1:102">
+    <row r="32" spans="1:113">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Update PCA analysis; add trials disconnecting PN2ITN with substituted baseline input
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="449">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1792,7 +1792,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>200 Hz</t>
+    <t>long_validate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Burst Hz</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2206,13 +2210,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DL59"/>
+  <dimension ref="A1:DN59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="CV3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DE12" sqref="DE12"/>
+      <selection pane="bottomRight" activeCell="DJ19" sqref="DJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2248,10 +2252,11 @@
     <col min="105" max="105" width="9" style="13"/>
     <col min="106" max="107" width="9" style="9"/>
     <col min="108" max="108" width="9" style="13"/>
-    <col min="110" max="116" width="9" style="7"/>
+    <col min="110" max="111" width="9" style="7"/>
+    <col min="112" max="113" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113">
+    <row r="1" spans="1:118">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2547,11 +2552,14 @@
       <c r="DG1" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="DI1" s="7" t="s">
+      <c r="DH1" s="13" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="2" spans="1:113">
+      <c r="DI1" s="13" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="2" spans="1:118">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2562,7 +2570,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:113">
+    <row r="3" spans="1:118">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2890,11 +2898,15 @@
       <c r="DG3" s="7">
         <v>1.9</v>
       </c>
-      <c r="DI3" s="7">
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:113">
+      <c r="DH3" s="13">
+        <v>2.74</v>
+      </c>
+      <c r="DI3" s="13">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="DN3" s="7"/>
+    </row>
+    <row r="4" spans="1:118">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3216,11 +3228,15 @@
       <c r="DG4" s="7">
         <v>1.7</v>
       </c>
-      <c r="DI4" s="7">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:113">
+      <c r="DH4" s="13">
+        <v>1.83</v>
+      </c>
+      <c r="DI4" s="13">
+        <v>1.68</v>
+      </c>
+      <c r="DN4" s="7"/>
+    </row>
+    <row r="5" spans="1:118">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3545,11 +3561,15 @@
       <c r="DG5" s="7">
         <v>2.61</v>
       </c>
-      <c r="DI5" s="7">
-        <v>2.58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:113">
+      <c r="DH5" s="13">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="DI5" s="13">
+        <v>3.06</v>
+      </c>
+      <c r="DN5" s="7"/>
+    </row>
+    <row r="6" spans="1:118">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3868,11 +3888,15 @@
       <c r="DG6" s="7">
         <v>1.78</v>
       </c>
-      <c r="DI6" s="7">
-        <v>1.66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:113">
+      <c r="DH6" s="13">
+        <v>1.59</v>
+      </c>
+      <c r="DI6" s="13">
+        <v>1.9</v>
+      </c>
+      <c r="DN6" s="7"/>
+    </row>
+    <row r="7" spans="1:118">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4197,11 +4221,15 @@
       <c r="DG7" s="7">
         <v>5.91</v>
       </c>
-      <c r="DI7" s="7">
-        <v>30.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:113">
+      <c r="DH7" s="13">
+        <v>28.4</v>
+      </c>
+      <c r="DI7" s="13">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="DN7" s="7"/>
+    </row>
+    <row r="8" spans="1:118">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -4520,11 +4548,15 @@
       <c r="DG8" s="7">
         <v>5.12</v>
       </c>
-      <c r="DI8" s="7">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:113">
+      <c r="DH8" s="13">
+        <v>37.1</v>
+      </c>
+      <c r="DI8" s="13">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="DN8" s="7"/>
+    </row>
+    <row r="9" spans="1:118">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4849,11 +4881,15 @@
       <c r="DG9" s="7">
         <v>11.6</v>
       </c>
-      <c r="DI9" s="7">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:113">
+      <c r="DH9" s="13">
+        <v>7.87</v>
+      </c>
+      <c r="DI9" s="13">
+        <v>15.6</v>
+      </c>
+      <c r="DN9" s="7"/>
+    </row>
+    <row r="10" spans="1:118">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -5172,11 +5208,15 @@
       <c r="DG10" s="7">
         <v>6.4</v>
       </c>
-      <c r="DI10" s="7">
-        <v>6.56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:113">
+      <c r="DH10" s="13">
+        <v>6.33</v>
+      </c>
+      <c r="DI10" s="13">
+        <v>14.4</v>
+      </c>
+      <c r="DN10" s="7"/>
+    </row>
+    <row r="11" spans="1:118">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5318,8 +5358,9 @@
       <c r="DG11" s="7">
         <v>41.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:113">
+      <c r="DN11" s="7"/>
+    </row>
+    <row r="12" spans="1:118">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -5458,8 +5499,9 @@
       <c r="DG12" s="7">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="13" spans="1:113">
+      <c r="DN12" s="7"/>
+    </row>
+    <row r="13" spans="1:118">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -5523,8 +5565,9 @@
       <c r="DF13" s="7">
         <v>40.299999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:113">
+      <c r="DN13" s="7"/>
+    </row>
+    <row r="14" spans="1:118">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -5588,16 +5631,31 @@
       <c r="DF14" s="7">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="15" spans="1:113">
+      <c r="DN14" s="7"/>
+    </row>
+    <row r="15" spans="1:118">
       <c r="DF15" s="7">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:113">
+      <c r="DH15" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="DI15" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="DN15" s="7"/>
+    </row>
+    <row r="16" spans="1:118">
       <c r="DF16" s="7">
         <v>0.5</v>
       </c>
+      <c r="DH16" s="13">
+        <v>200</v>
+      </c>
+      <c r="DI16" s="13">
+        <v>60</v>
+      </c>
+      <c r="DN16" s="7"/>
     </row>
     <row r="17" spans="1:113">
       <c r="A17" s="3" t="s">
@@ -5898,7 +5956,7 @@
       <c r="CX19" s="5">
         <v>1.53</v>
       </c>
-      <c r="DI19" s="7">
+      <c r="DH19" s="13">
         <v>1.53</v>
       </c>
     </row>
@@ -5999,15 +6057,15 @@
       <c r="CX20" s="5">
         <v>2.2240000000000002</v>
       </c>
+      <c r="DI20" s="13">
+        <v>2.2240000000000002</v>
+      </c>
     </row>
     <row r="21" spans="1:113">
       <c r="C21" t="s">
         <v>32</v>
       </c>
       <c r="CM21" s="7"/>
-      <c r="DI21" s="7" t="s">
-        <v>447</v>
-      </c>
     </row>
     <row r="22" spans="1:113">
       <c r="A22" s="3" t="s">
@@ -6161,8 +6219,11 @@
       <c r="CT26" s="5">
         <v>8.5</v>
       </c>
-      <c r="DI26" s="7">
+      <c r="DH26" s="13">
         <v>0</v>
+      </c>
+      <c r="DI26" s="13">
+        <v>8.5</v>
       </c>
     </row>
     <row r="27" spans="1:113">
@@ -6206,8 +6267,11 @@
       <c r="CT27" s="5">
         <v>1.88</v>
       </c>
-      <c r="DI27" s="7">
+      <c r="DH27" s="13">
         <v>0</v>
+      </c>
+      <c r="DI27" s="13">
+        <v>1.88</v>
       </c>
     </row>
     <row r="28" spans="1:113">
@@ -6237,6 +6301,9 @@
       <c r="CT28" s="5">
         <v>1.26</v>
       </c>
+      <c r="DI28" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:113">
       <c r="B29" s="3" t="s">
@@ -6264,6 +6331,9 @@
       <c r="CM29" s="7"/>
       <c r="CT29" s="5">
         <v>0.53</v>
+      </c>
+      <c r="DI29" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:113">

</xml_diff>

<commit_message>
Add validation without STP
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="466">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1797,6 +1797,74 @@
   </si>
   <si>
     <t>Burst Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove PN2FSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove PN2LTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bursts of poisson</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input to FSI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input to LTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_no_STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remove all STP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time constants</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust U to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>match baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>synaptic weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_no_STP_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>using firing rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of all units</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use mean firing rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2210,13 +2278,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DN59"/>
+  <dimension ref="A1:DR64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CV3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CX3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DJ19" sqref="DJ19"/>
+      <selection pane="bottomRight" activeCell="DP13" sqref="DP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2253,10 +2321,13 @@
     <col min="106" max="107" width="9" style="9"/>
     <col min="108" max="108" width="9" style="13"/>
     <col min="110" max="111" width="9" style="7"/>
-    <col min="112" max="113" width="9" style="13"/>
+    <col min="113" max="113" width="9" style="13"/>
+    <col min="115" max="115" width="9" style="13"/>
+    <col min="117" max="117" width="9" style="9"/>
+    <col min="119" max="120" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118">
+    <row r="1" spans="1:122">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2552,14 +2623,23 @@
       <c r="DG1" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="DH1" s="13" t="s">
+      <c r="DI1" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="DI1" s="13" t="s">
+      <c r="DK1" s="13" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="2" spans="1:118">
+      <c r="DM1" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="DO1" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="DP1" s="13" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:122">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2570,7 +2650,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:118">
+    <row r="3" spans="1:122">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2898,15 +2978,30 @@
       <c r="DG3" s="7">
         <v>1.9</v>
       </c>
-      <c r="DH3" s="13">
+      <c r="DI3" s="13">
         <v>2.74</v>
       </c>
-      <c r="DI3" s="13">
+      <c r="DJ3">
+        <v>2.61</v>
+      </c>
+      <c r="DK3" s="13">
         <v>2.0499999999999998</v>
       </c>
-      <c r="DN3" s="7"/>
-    </row>
-    <row r="4" spans="1:118">
+      <c r="DM3" s="9">
+        <v>1.91</v>
+      </c>
+      <c r="DN3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="DO3" s="13">
+        <v>3.03</v>
+      </c>
+      <c r="DP3" s="13">
+        <v>3.05</v>
+      </c>
+      <c r="DR3" s="7"/>
+    </row>
+    <row r="4" spans="1:122">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3228,15 +3323,30 @@
       <c r="DG4" s="7">
         <v>1.7</v>
       </c>
-      <c r="DH4" s="13">
+      <c r="DI4" s="13">
         <v>1.83</v>
       </c>
-      <c r="DI4" s="13">
+      <c r="DJ4">
+        <v>1.84</v>
+      </c>
+      <c r="DK4" s="13">
         <v>1.68</v>
       </c>
-      <c r="DN4" s="7"/>
-    </row>
-    <row r="5" spans="1:118">
+      <c r="DM4" s="9">
+        <v>1.82</v>
+      </c>
+      <c r="DN4">
+        <v>1.81</v>
+      </c>
+      <c r="DO4" s="13">
+        <v>1.84</v>
+      </c>
+      <c r="DP4" s="13">
+        <v>1.81</v>
+      </c>
+      <c r="DR4" s="7"/>
+    </row>
+    <row r="5" spans="1:122">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3561,15 +3671,30 @@
       <c r="DG5" s="7">
         <v>2.61</v>
       </c>
-      <c r="DH5" s="13">
+      <c r="DI5" s="13">
         <v>2.4300000000000002</v>
       </c>
-      <c r="DI5" s="13">
+      <c r="DJ5">
+        <v>2.74</v>
+      </c>
+      <c r="DK5" s="13">
         <v>3.06</v>
       </c>
-      <c r="DN5" s="7"/>
-    </row>
-    <row r="6" spans="1:118">
+      <c r="DM5" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="DN5">
+        <v>1.05</v>
+      </c>
+      <c r="DO5" s="13">
+        <v>1.97</v>
+      </c>
+      <c r="DP5" s="13">
+        <v>2.11</v>
+      </c>
+      <c r="DR5" s="7"/>
+    </row>
+    <row r="6" spans="1:122">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -3888,15 +4013,30 @@
       <c r="DG6" s="7">
         <v>1.78</v>
       </c>
-      <c r="DH6" s="13">
+      <c r="DI6" s="13">
         <v>1.59</v>
       </c>
-      <c r="DI6" s="13">
+      <c r="DJ6">
+        <v>1.73</v>
+      </c>
+      <c r="DK6" s="13">
         <v>1.9</v>
       </c>
-      <c r="DN6" s="7"/>
-    </row>
-    <row r="7" spans="1:118">
+      <c r="DM6" s="9">
+        <v>1.37</v>
+      </c>
+      <c r="DN6">
+        <v>1.2</v>
+      </c>
+      <c r="DO6" s="13">
+        <v>1.39</v>
+      </c>
+      <c r="DP6" s="13">
+        <v>1.39</v>
+      </c>
+      <c r="DR6" s="7"/>
+    </row>
+    <row r="7" spans="1:122">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4221,15 +4361,30 @@
       <c r="DG7" s="7">
         <v>5.91</v>
       </c>
-      <c r="DH7" s="13">
+      <c r="DI7" s="13">
         <v>28.4</v>
       </c>
-      <c r="DI7" s="13">
+      <c r="DJ7">
+        <v>16.3</v>
+      </c>
+      <c r="DK7" s="13">
         <v>4.1399999999999997</v>
       </c>
-      <c r="DN7" s="7"/>
-    </row>
-    <row r="8" spans="1:118">
+      <c r="DM7" s="9">
+        <v>7.42</v>
+      </c>
+      <c r="DN7">
+        <v>9.49</v>
+      </c>
+      <c r="DO7" s="13">
+        <v>16.8</v>
+      </c>
+      <c r="DP7" s="13">
+        <v>17.5</v>
+      </c>
+      <c r="DR7" s="7"/>
+    </row>
+    <row r="8" spans="1:122">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -4548,15 +4703,30 @@
       <c r="DG8" s="7">
         <v>5.12</v>
       </c>
-      <c r="DH8" s="13">
+      <c r="DI8" s="13">
         <v>37.1</v>
       </c>
-      <c r="DI8" s="13">
+      <c r="DJ8">
+        <v>26.7</v>
+      </c>
+      <c r="DK8" s="13">
         <v>5.0199999999999996</v>
       </c>
-      <c r="DN8" s="7"/>
-    </row>
-    <row r="9" spans="1:118">
+      <c r="DM8" s="9">
+        <v>6.4</v>
+      </c>
+      <c r="DN8">
+        <v>7.22</v>
+      </c>
+      <c r="DO8" s="13">
+        <v>11.1</v>
+      </c>
+      <c r="DP8" s="13">
+        <v>11.4</v>
+      </c>
+      <c r="DR8" s="7"/>
+    </row>
+    <row r="9" spans="1:122">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4881,15 +5051,30 @@
       <c r="DG9" s="7">
         <v>11.6</v>
       </c>
-      <c r="DH9" s="13">
+      <c r="DI9" s="13">
         <v>7.87</v>
       </c>
-      <c r="DI9" s="13">
+      <c r="DJ9">
+        <v>9.36</v>
+      </c>
+      <c r="DK9" s="13">
         <v>15.6</v>
       </c>
-      <c r="DN9" s="7"/>
-    </row>
-    <row r="10" spans="1:118">
+      <c r="DM9" s="9">
+        <v>5.04</v>
+      </c>
+      <c r="DN9">
+        <v>3.37</v>
+      </c>
+      <c r="DO9" s="13">
+        <v>4.97</v>
+      </c>
+      <c r="DP9" s="13">
+        <v>4.96</v>
+      </c>
+      <c r="DR9" s="7"/>
+    </row>
+    <row r="10" spans="1:122">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -5208,15 +5393,30 @@
       <c r="DG10" s="7">
         <v>6.4</v>
       </c>
-      <c r="DH10" s="13">
+      <c r="DI10" s="13">
         <v>6.33</v>
       </c>
-      <c r="DI10" s="13">
+      <c r="DJ10">
+        <v>6.53</v>
+      </c>
+      <c r="DK10" s="13">
         <v>14.4</v>
       </c>
-      <c r="DN10" s="7"/>
-    </row>
-    <row r="11" spans="1:118">
+      <c r="DM10" s="9">
+        <v>5.94</v>
+      </c>
+      <c r="DN10">
+        <v>5.22</v>
+      </c>
+      <c r="DO10" s="13">
+        <v>5.97</v>
+      </c>
+      <c r="DP10" s="13">
+        <v>5.94</v>
+      </c>
+      <c r="DR10" s="7"/>
+    </row>
+    <row r="11" spans="1:122">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5358,9 +5558,15 @@
       <c r="DG11" s="7">
         <v>41.4</v>
       </c>
-      <c r="DN11" s="7"/>
-    </row>
-    <row r="12" spans="1:118">
+      <c r="DO11" s="13">
+        <v>40</v>
+      </c>
+      <c r="DP11" s="13">
+        <v>40.4</v>
+      </c>
+      <c r="DR11" s="7"/>
+    </row>
+    <row r="12" spans="1:122">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -5499,9 +5705,15 @@
       <c r="DG12" s="7">
         <v>0.59</v>
       </c>
-      <c r="DN12" s="7"/>
-    </row>
-    <row r="13" spans="1:118">
+      <c r="DO12" s="13">
+        <v>0.92</v>
+      </c>
+      <c r="DP12" s="13">
+        <v>1.01</v>
+      </c>
+      <c r="DR12" s="7"/>
+    </row>
+    <row r="13" spans="1:122">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -5565,9 +5777,9 @@
       <c r="DF13" s="7">
         <v>40.299999999999997</v>
       </c>
-      <c r="DN13" s="7"/>
-    </row>
-    <row r="14" spans="1:118">
+      <c r="DR13" s="7"/>
+    </row>
+    <row r="14" spans="1:122">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -5631,33 +5843,36 @@
       <c r="DF14" s="7">
         <v>0.59</v>
       </c>
-      <c r="DN14" s="7"/>
-    </row>
-    <row r="15" spans="1:118">
+      <c r="DR14" s="7"/>
+    </row>
+    <row r="15" spans="1:122">
       <c r="DF15" s="7">
         <v>47</v>
       </c>
-      <c r="DH15" s="13" t="s">
-        <v>448</v>
-      </c>
       <c r="DI15" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="DN15" s="7"/>
-    </row>
-    <row r="16" spans="1:118">
+      <c r="DK15" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="DR15" s="7"/>
+    </row>
+    <row r="16" spans="1:122">
       <c r="DF16" s="7">
         <v>0.5</v>
       </c>
-      <c r="DH16" s="13">
+      <c r="DI16" s="13">
         <v>200</v>
       </c>
-      <c r="DI16" s="13">
+      <c r="DJ16">
+        <v>160</v>
+      </c>
+      <c r="DK16" s="13">
         <v>60</v>
       </c>
-      <c r="DN16" s="7"/>
-    </row>
-    <row r="17" spans="1:113">
+      <c r="DR16" s="7"/>
+    </row>
+    <row r="17" spans="1:117">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -5754,7 +5969,7 @@
         <v>8.01</v>
       </c>
     </row>
-    <row r="18" spans="1:113">
+    <row r="18" spans="1:117">
       <c r="B18" s="3" t="s">
         <v>5</v>
       </c>
@@ -5828,7 +6043,7 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="19" spans="1:113">
+    <row r="19" spans="1:117">
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
@@ -5956,11 +6171,11 @@
       <c r="CX19" s="5">
         <v>1.53</v>
       </c>
-      <c r="DH19" s="13">
+      <c r="DI19" s="13">
         <v>1.53</v>
       </c>
     </row>
-    <row r="20" spans="1:113">
+    <row r="20" spans="1:117">
       <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
@@ -6057,17 +6272,17 @@
       <c r="CX20" s="5">
         <v>2.2240000000000002</v>
       </c>
-      <c r="DI20" s="13">
+      <c r="DK20" s="13">
         <v>2.2240000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:113">
+    <row r="21" spans="1:117">
       <c r="C21" t="s">
         <v>32</v>
       </c>
       <c r="CM21" s="7"/>
     </row>
-    <row r="22" spans="1:113">
+    <row r="22" spans="1:117">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -6097,7 +6312,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="23" spans="1:113">
+    <row r="23" spans="1:117">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
@@ -6124,7 +6339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:113">
+    <row r="24" spans="1:117">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
@@ -6151,7 +6366,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:113">
+    <row r="25" spans="1:117">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
@@ -6178,7 +6393,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:113">
+    <row r="26" spans="1:117">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
@@ -6219,14 +6434,14 @@
       <c r="CT26" s="5">
         <v>8.5</v>
       </c>
-      <c r="DH26" s="13">
+      <c r="DI26" s="13">
         <v>0</v>
       </c>
-      <c r="DI26" s="13">
+      <c r="DK26" s="13">
         <v>8.5</v>
       </c>
     </row>
-    <row r="27" spans="1:113">
+    <row r="27" spans="1:117">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
@@ -6267,14 +6482,14 @@
       <c r="CT27" s="5">
         <v>1.88</v>
       </c>
-      <c r="DH27" s="13">
+      <c r="DI27" s="13">
         <v>0</v>
       </c>
-      <c r="DI27" s="13">
+      <c r="DK27" s="13">
         <v>1.88</v>
       </c>
     </row>
-    <row r="28" spans="1:113">
+    <row r="28" spans="1:117">
       <c r="B28" s="3" t="s">
         <v>23</v>
       </c>
@@ -6301,11 +6516,14 @@
       <c r="CT28" s="5">
         <v>1.26</v>
       </c>
-      <c r="DI28" s="13">
+      <c r="DK28" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:113">
+      <c r="DM28" s="9">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:117">
       <c r="B29" s="3" t="s">
         <v>24</v>
       </c>
@@ -6332,11 +6550,14 @@
       <c r="CT29" s="5">
         <v>0.53</v>
       </c>
-      <c r="DI29" s="13">
+      <c r="DK29" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:113">
+      <c r="DM29" s="9">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:117">
       <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
@@ -6361,7 +6582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:113">
+    <row r="31" spans="1:117">
       <c r="B31" s="3" t="s">
         <v>26</v>
       </c>
@@ -6386,7 +6607,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="32" spans="1:113">
+    <row r="32" spans="1:117">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -6842,7 +7063,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="49" spans="1:101">
+    <row r="49" spans="1:118">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -6862,7 +7083,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="51" spans="1:101">
+    <row r="51" spans="1:118">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -6884,8 +7105,11 @@
       <c r="CT51" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="52" spans="1:101">
+      <c r="DM51" s="9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="52" spans="1:118">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -6919,8 +7143,11 @@
       <c r="CT52" s="5">
         <v>400</v>
       </c>
-    </row>
-    <row r="53" spans="1:101">
+      <c r="DM52" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:118">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -6951,8 +7178,11 @@
       <c r="CT53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:101">
+      <c r="DM53" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:118">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -6972,8 +7202,11 @@
       <c r="CT54" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="55" spans="1:101">
+      <c r="DM54" s="9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="55" spans="1:118">
       <c r="D55" s="11">
         <v>25</v>
       </c>
@@ -7001,8 +7234,11 @@
       <c r="CT55" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:101">
+      <c r="DM55" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:118">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -7033,8 +7269,11 @@
       <c r="CT56" s="5">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:101">
+      <c r="DM56" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:118">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -7050,13 +7289,65 @@
       <c r="CW58" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="59" spans="1:101">
+      <c r="DI58" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="DK58" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="DM58" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="DN58" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="59" spans="1:118">
       <c r="L59" t="s">
         <v>350</v>
       </c>
       <c r="CW59" t="s">
         <v>436</v>
+      </c>
+      <c r="DI59" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="DK59" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="DM59" s="9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="60" spans="1:118">
+      <c r="DI60" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="DK60" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="DM60" s="9" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="61" spans="1:118">
+      <c r="DM61" s="9" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="62" spans="1:118">
+      <c r="DM62" s="9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:118">
+      <c r="DM63" s="9" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="64" spans="1:118">
+      <c r="DM64" s="9" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove outdated codes; Add script for scaling synaptic weights of PN assemblies and simulation config with scaled network
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="476">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1865,6 +1865,46 @@
   </si>
   <si>
     <t>Use mean firing rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scale synaptic weight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>for PN assemblies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same assembly has</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>different assemblies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2x the mean weights of</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_syn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_rand_syn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_rand_syn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_div_syn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_div_syn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2278,13 +2318,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DR64"/>
+  <dimension ref="A1:DX64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CX3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="DD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DP13" sqref="DP13"/>
+      <selection pane="bottomRight" activeCell="DR12" sqref="DR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2325,9 +2365,12 @@
     <col min="115" max="115" width="9" style="13"/>
     <col min="117" max="117" width="9" style="9"/>
     <col min="119" max="120" width="9" style="13"/>
+    <col min="122" max="122" width="9" style="9"/>
+    <col min="123" max="126" width="9" style="13"/>
+    <col min="127" max="128" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:122">
+    <row r="1" spans="1:126">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2638,8 +2681,23 @@
       <c r="DP1" s="13" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="2" spans="1:122">
+      <c r="DR1" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="DS1" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="DT1" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="DU1" s="13" t="s">
+        <v>474</v>
+      </c>
+      <c r="DV1" s="13" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="2" spans="1:126">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2650,7 +2708,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:122">
+    <row r="3" spans="1:126">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2999,9 +3057,11 @@
       <c r="DP3" s="13">
         <v>3.05</v>
       </c>
-      <c r="DR3" s="7"/>
-    </row>
-    <row r="4" spans="1:122">
+      <c r="DR3" s="9">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:126">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3344,9 +3404,11 @@
       <c r="DP4" s="13">
         <v>1.81</v>
       </c>
-      <c r="DR4" s="7"/>
-    </row>
-    <row r="5" spans="1:122">
+      <c r="DR4" s="9">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:126">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -3692,9 +3754,11 @@
       <c r="DP5" s="13">
         <v>2.11</v>
       </c>
-      <c r="DR5" s="7"/>
-    </row>
-    <row r="6" spans="1:122">
+      <c r="DR5" s="9">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:126">
       <c r="C6" s="12">
         <v>1.1000000000000001</v>
       </c>
@@ -4034,9 +4098,11 @@
       <c r="DP6" s="13">
         <v>1.39</v>
       </c>
-      <c r="DR6" s="7"/>
-    </row>
-    <row r="7" spans="1:122">
+      <c r="DR6" s="9">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:126">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4382,9 +4448,11 @@
       <c r="DP7" s="13">
         <v>17.5</v>
       </c>
-      <c r="DR7" s="7"/>
-    </row>
-    <row r="8" spans="1:122">
+      <c r="DR7" s="9">
+        <v>7.43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:126">
       <c r="C8" s="12">
         <v>6.4</v>
       </c>
@@ -4724,9 +4792,11 @@
       <c r="DP8" s="13">
         <v>11.4</v>
       </c>
-      <c r="DR8" s="7"/>
-    </row>
-    <row r="9" spans="1:122">
+      <c r="DR8" s="9">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:126">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -5072,9 +5142,11 @@
       <c r="DP9" s="13">
         <v>4.96</v>
       </c>
-      <c r="DR9" s="7"/>
-    </row>
-    <row r="10" spans="1:122">
+      <c r="DR9" s="9">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:126">
       <c r="C10" s="12">
         <v>5</v>
       </c>
@@ -5414,9 +5486,11 @@
       <c r="DP10" s="13">
         <v>5.94</v>
       </c>
-      <c r="DR10" s="7"/>
-    </row>
-    <row r="11" spans="1:122">
+      <c r="DR10" s="9">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:126">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -5564,9 +5638,8 @@
       <c r="DP11" s="13">
         <v>40.4</v>
       </c>
-      <c r="DR11" s="7"/>
-    </row>
-    <row r="12" spans="1:122">
+    </row>
+    <row r="12" spans="1:126">
       <c r="B12" s="3" t="s">
         <v>44</v>
       </c>
@@ -5711,9 +5784,8 @@
       <c r="DP12" s="13">
         <v>1.01</v>
       </c>
-      <c r="DR12" s="7"/>
-    </row>
-    <row r="13" spans="1:122">
+    </row>
+    <row r="13" spans="1:126">
       <c r="N13">
         <v>37.1</v>
       </c>
@@ -5777,9 +5849,8 @@
       <c r="DF13" s="7">
         <v>40.299999999999997</v>
       </c>
-      <c r="DR13" s="7"/>
-    </row>
-    <row r="14" spans="1:122">
+    </row>
+    <row r="14" spans="1:126">
       <c r="N14">
         <v>0.62</v>
       </c>
@@ -5843,9 +5914,8 @@
       <c r="DF14" s="7">
         <v>0.59</v>
       </c>
-      <c r="DR14" s="7"/>
-    </row>
-    <row r="15" spans="1:122">
+    </row>
+    <row r="15" spans="1:126">
       <c r="DF15" s="7">
         <v>47</v>
       </c>
@@ -5855,9 +5925,8 @@
       <c r="DK15" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="DR15" s="7"/>
-    </row>
-    <row r="16" spans="1:122">
+    </row>
+    <row r="16" spans="1:126">
       <c r="DF16" s="7">
         <v>0.5</v>
       </c>
@@ -5870,7 +5939,6 @@
       <c r="DK16" s="13">
         <v>60</v>
       </c>
-      <c r="DR16" s="7"/>
     </row>
     <row r="17" spans="1:117">
       <c r="A17" s="3" t="s">
@@ -7063,7 +7131,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="49" spans="1:118">
+    <row r="49" spans="1:122">
       <c r="B49" s="3" t="s">
         <v>24</v>
       </c>
@@ -7083,7 +7151,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="51" spans="1:118">
+    <row r="51" spans="1:122">
       <c r="A51" s="3" t="s">
         <v>281</v>
       </c>
@@ -7109,7 +7177,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="1:118">
+    <row r="52" spans="1:122">
       <c r="A52" s="3" t="s">
         <v>282</v>
       </c>
@@ -7147,7 +7215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:118">
+    <row r="53" spans="1:122">
       <c r="A53" s="3" t="s">
         <v>283</v>
       </c>
@@ -7182,7 +7250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:118">
+    <row r="54" spans="1:122">
       <c r="B54" s="3" t="s">
         <v>280</v>
       </c>
@@ -7206,7 +7274,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:118">
+    <row r="55" spans="1:122">
       <c r="D55" s="11">
         <v>25</v>
       </c>
@@ -7238,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:118">
+    <row r="56" spans="1:122">
       <c r="D56" s="11">
         <v>100</v>
       </c>
@@ -7273,7 +7341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:118">
+    <row r="58" spans="1:122">
       <c r="A58" s="3" t="s">
         <v>37</v>
       </c>
@@ -7301,8 +7369,11 @@
       <c r="DN58" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="59" spans="1:118">
+      <c r="DR58" s="9" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="59" spans="1:122">
       <c r="L59" t="s">
         <v>350</v>
       </c>
@@ -7318,8 +7389,11 @@
       <c r="DM59" s="9" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="60" spans="1:118">
+      <c r="DR59" s="9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="60" spans="1:122">
       <c r="DI60" s="13" t="s">
         <v>452</v>
       </c>
@@ -7329,23 +7403,32 @@
       <c r="DM60" s="9" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="61" spans="1:118">
+      <c r="DR60" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="61" spans="1:122">
       <c r="DM61" s="9" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="62" spans="1:118">
+      <c r="DR61" s="9" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="62" spans="1:122">
       <c r="DM62" s="9" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="63" spans="1:118">
+      <c r="DR62" s="9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="63" spans="1:122">
       <c r="DM63" s="9" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="64" spans="1:118">
+    <row r="64" spans="1:122">
       <c r="DM64" s="9" t="s">
         <v>464</v>
       </c>

</xml_diff>

<commit_message>
Add results of short/long pulses using network with scaled synaptic weights of PN assemblies
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -2324,7 +2324,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="DD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DR12" sqref="DR12"/>
+      <selection pane="bottomRight" activeCell="DU33" sqref="DU33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3060,6 +3060,18 @@
       <c r="DR3" s="9">
         <v>1.9</v>
       </c>
+      <c r="DS3" s="13">
+        <v>2.88</v>
+      </c>
+      <c r="DT3" s="13">
+        <v>1.97</v>
+      </c>
+      <c r="DU3" s="13">
+        <v>2.94</v>
+      </c>
+      <c r="DV3" s="13">
+        <v>1.96</v>
+      </c>
     </row>
     <row r="4" spans="1:126">
       <c r="A4" s="3" t="s">
@@ -3407,6 +3419,18 @@
       <c r="DR4" s="9">
         <v>1.82</v>
       </c>
+      <c r="DS4" s="13">
+        <v>1.86</v>
+      </c>
+      <c r="DT4" s="13">
+        <v>1.57</v>
+      </c>
+      <c r="DU4" s="13">
+        <v>1.87</v>
+      </c>
+      <c r="DV4" s="13">
+        <v>1.53</v>
+      </c>
     </row>
     <row r="5" spans="1:126">
       <c r="B5" s="3" t="s">
@@ -3757,6 +3781,18 @@
       <c r="DR5" s="9">
         <v>1.3</v>
       </c>
+      <c r="DS5" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="DT5" s="13">
+        <v>2.82</v>
+      </c>
+      <c r="DU5" s="13">
+        <v>2.36</v>
+      </c>
+      <c r="DV5" s="13">
+        <v>2.81</v>
+      </c>
     </row>
     <row r="6" spans="1:126">
       <c r="C6" s="12">
@@ -4101,6 +4137,18 @@
       <c r="DR6" s="9">
         <v>1.37</v>
       </c>
+      <c r="DS6" s="13">
+        <v>1.51</v>
+      </c>
+      <c r="DT6" s="13">
+        <v>1.72</v>
+      </c>
+      <c r="DU6" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="DV6" s="13">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="7" spans="1:126">
       <c r="B7" s="3" t="s">
@@ -4451,6 +4499,18 @@
       <c r="DR7" s="9">
         <v>7.43</v>
       </c>
+      <c r="DS7" s="13">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="DT7" s="13">
+        <v>4.49</v>
+      </c>
+      <c r="DU7" s="13">
+        <v>18.3</v>
+      </c>
+      <c r="DV7" s="13">
+        <v>4.32</v>
+      </c>
     </row>
     <row r="8" spans="1:126">
       <c r="C8" s="12">
@@ -4795,6 +4855,18 @@
       <c r="DR8" s="9">
         <v>6.33</v>
       </c>
+      <c r="DS8" s="13">
+        <v>11.1</v>
+      </c>
+      <c r="DT8" s="13">
+        <v>4.18</v>
+      </c>
+      <c r="DU8" s="13">
+        <v>11.3</v>
+      </c>
+      <c r="DV8" s="13">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="9" spans="1:126">
       <c r="B9" s="3" t="s">
@@ -5145,6 +5217,18 @@
       <c r="DR9" s="9">
         <v>5.01</v>
       </c>
+      <c r="DS9" s="13">
+        <v>6.98</v>
+      </c>
+      <c r="DT9" s="13">
+        <v>14.3</v>
+      </c>
+      <c r="DU9" s="13">
+        <v>7.3</v>
+      </c>
+      <c r="DV9" s="13">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:126">
       <c r="C10" s="12">
@@ -5489,6 +5573,18 @@
       <c r="DR10" s="9">
         <v>5.89</v>
       </c>
+      <c r="DS10" s="13">
+        <v>6.37</v>
+      </c>
+      <c r="DT10" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="DU10" s="13">
+        <v>6.44</v>
+      </c>
+      <c r="DV10" s="13">
+        <v>7.05</v>
+      </c>
     </row>
     <row r="11" spans="1:126">
       <c r="A11" s="3" t="s">
@@ -5638,6 +5734,18 @@
       <c r="DP11" s="13">
         <v>40.4</v>
       </c>
+      <c r="DS11" s="13">
+        <v>38</v>
+      </c>
+      <c r="DT11" s="13">
+        <v>17.8</v>
+      </c>
+      <c r="DU11" s="13">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="DV11" s="13">
+        <v>17.7</v>
+      </c>
     </row>
     <row r="12" spans="1:126">
       <c r="B12" s="3" t="s">
@@ -5784,6 +5892,18 @@
       <c r="DP12" s="13">
         <v>1.01</v>
       </c>
+      <c r="DS12" s="13">
+        <v>0.51</v>
+      </c>
+      <c r="DT12" s="13">
+        <v>0.96</v>
+      </c>
+      <c r="DU12" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="DV12" s="13">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:126">
       <c r="N13">
@@ -5849,6 +5969,12 @@
       <c r="DF13" s="7">
         <v>40.299999999999997</v>
       </c>
+      <c r="DT13" s="13">
+        <v>38</v>
+      </c>
+      <c r="DV13" s="13">
+        <v>38.1</v>
+      </c>
     </row>
     <row r="14" spans="1:126">
       <c r="N14">
@@ -5913,6 +6039,12 @@
       </c>
       <c r="DF14" s="7">
         <v>0.59</v>
+      </c>
+      <c r="DT14" s="13">
+        <v>0.52</v>
+      </c>
+      <c r="DV14" s="13">
+        <v>0.43</v>
       </c>
     </row>
     <row r="15" spans="1:126">

</xml_diff>